<commit_message>
Docs & BOM: Excluded tax
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -153,16 +153,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">DigiKey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">505-LT3750EMS#PBF-ND</t>
+    <t xml:space="preserve">Farnell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANALOG DEVICES LT3750EMS#TRPBF</t>
   </si>
   <si>
     <t xml:space="preserve">Analog-devices</t>
   </si>
   <si>
-    <t xml:space="preserve">LT3750EMS#PBF</t>
+    <t xml:space="preserve">LT3750EMS#TRPBF</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitor charging controller for kicker
@@ -233,9 +233,6 @@
   </si>
   <si>
     <t xml:space="preserve">BROADCOM AEDB-9140-A13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farnell</t>
   </si>
   <si>
     <t xml:space="preserve">BROADCOM</t>
@@ -902,22 +899,22 @@
   </sheetPr>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="37.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="44.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="116.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="35.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="41.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,11 +982,11 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="n">
-        <v>371</v>
+        <v>297</v>
       </c>
       <c r="I3" s="2" t="n">
         <f aca="false">C3*H3</f>
-        <v>1484</v>
+        <v>1188</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>13</v>
@@ -1017,11 +1014,11 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="n">
-        <v>289</v>
+        <v>215.4</v>
       </c>
       <c r="I4" s="2" t="n">
         <f aca="false">C4*H4</f>
-        <v>1156</v>
+        <v>861.6</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
@@ -1047,11 +1044,11 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="9" t="n">
-        <v>336</v>
+        <v>268.8</v>
       </c>
       <c r="I5" s="2" t="n">
         <f aca="false">C5*H5</f>
-        <v>1344</v>
+        <v>1075.2</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
@@ -1077,11 +1074,11 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="n">
-        <v>184</v>
+        <v>147.2</v>
       </c>
       <c r="I6" s="2" t="n">
         <f aca="false">C6*H6</f>
-        <v>920</v>
+        <v>736</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>13</v>
@@ -1107,11 +1104,11 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="n">
-        <v>193.51</v>
+        <v>154.808</v>
       </c>
       <c r="I7" s="2" t="n">
         <f aca="false">H7*C7</f>
-        <v>774.04</v>
+        <v>619.232</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>13</v>
@@ -1135,11 +1132,11 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="n">
-        <v>254</v>
+        <v>203.2</v>
       </c>
       <c r="I8" s="2" t="n">
         <f aca="false">C8*H8</f>
-        <v>254</v>
+        <v>203.2</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>13</v>
@@ -1169,11 +1166,11 @@
         <v>36</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>439</v>
+        <v>351.2</v>
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">C9*H9</f>
-        <v>439</v>
+        <v>351.2</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
@@ -1198,10 +1195,12 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="n">
+        <v>359.2</v>
+      </c>
       <c r="I10" s="2" t="n">
         <f aca="false">C10*H10</f>
-        <v>0</v>
+        <v>359.2</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>13</v>
@@ -1231,11 +1230,11 @@
         <v>44</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>120</v>
+        <v>60.14</v>
       </c>
       <c r="I11" s="2" t="n">
         <f aca="false">C11*H11</f>
-        <v>120</v>
+        <v>60.14</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>13</v>
@@ -1439,11 +1438,11 @@
         <v>62</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>247.94</v>
+        <v>198.352</v>
       </c>
       <c r="I20" s="2" t="n">
         <f aca="false">C20*H20</f>
-        <v>991.76</v>
+        <v>793.408</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>13</v>
@@ -1461,43 +1460,43 @@
         <v>24</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="H21" s="2" t="n">
-        <v>386.25</v>
+        <v>309</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">C21*H21</f>
-        <v>9270</v>
+        <v>7416</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>2536030320001</v>
@@ -1513,13 +1512,13 @@
         <v>13</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -1528,13 +1527,13 @@
         <v>59</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="H23" s="2" t="n">
         <v>605.13</v>
@@ -1547,12 +1546,12 @@
         <v>13</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1601,7 +1600,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1616,7 +1615,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1627,13 +1626,13 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1644,13 +1643,13 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1661,13 +1660,13 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1684,7 +1683,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1700,7 +1699,7 @@
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1749,54 +1748,54 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H34" s="2" t="n">
         <v>262.83</v>
       </c>
       <c r="I34" s="2" t="n">
         <f aca="false">C34*H34</f>
-        <v>788.49</v>
+        <v>1576.98</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
       <c r="B35" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>5901259432770</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="H35" s="2" t="n">
         <v>237</v>
@@ -1813,7 +1812,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>1</v>
@@ -1825,75 +1824,75 @@
         <v>65193</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="H36" s="2" t="n">
-        <v>219</v>
+        <v>175.2</v>
       </c>
       <c r="I36" s="2" t="n">
         <f aca="false">C36*H36</f>
-        <v>219</v>
+        <v>175.2</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="14" t="n">
         <f aca="false">SUM(I3,I6,I9,I11,I19,I23,I36)</f>
-        <v>4684.73</v>
+        <v>4013.27</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,7 +1900,7 @@
         <v>46</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F43" s="10"/>
     </row>
@@ -1912,37 +1911,37 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1964,7 +1963,7 @@
     <hyperlink ref="D9" r:id="rId8" display="Elefun"/>
     <hyperlink ref="F9" r:id="rId9" display="GNB"/>
     <hyperlink ref="D10" r:id="rId10" display="Droneit"/>
-    <hyperlink ref="D11" r:id="rId11" display="DigiKey"/>
+    <hyperlink ref="D11" r:id="rId11" display="Farnell"/>
     <hyperlink ref="F11" r:id="rId12" display="Analog-devices"/>
     <hyperlink ref="D19" r:id="rId13" display="Symmetry Electronics"/>
     <hyperlink ref="F19" r:id="rId14" location="documents" display="iC-Haus"/>

</xml_diff>

<commit_message>
Added a few comments and additional retailers based on the feedback we reveived from Henrik Falk.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_09976BEB9036F2153D1B5AD4644BDFF101C84B38" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{943A5C23-BDC2-433C-B0B1-5283EC31E24D}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_09976BEB9036F2153D1B5AD4644BDFF101C84B38" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D5C578D1-B026-49CB-9BC2-FF18964BB5C6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,16 +571,17 @@
     <t>Adafruit</t>
   </si>
   <si>
+    <t>IR Break Beam 3mm LEDs</t>
+  </si>
+  <si>
+    <t>Adafruit 3mm</t>
+  </si>
+  <si>
     <t>This is the better option since the emitter and 
 receiver might get "out of sight" after a collision.
 The risk of that happening is smaller if the beam 
-have a greater diameter.</t>
-  </si>
-  <si>
-    <t>IR Break Beam 3mm LEDs</t>
-  </si>
-  <si>
-    <t>Adafruit 3mm</t>
+have a greater diameter.
+These are sold at electro:kit</t>
   </si>
 </sst>
 </file>
@@ -740,15 +741,6 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -775,6 +767,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -994,1431 +995,1431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>9392000008</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
         <v>297</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <f>C4*H4</f>
         <v>1188</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
         <v>215.4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <f>C5*H5</f>
         <v>861.6</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>54896</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="11">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="8">
         <v>268.8</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <f>C6*H6</f>
         <v>1075.2</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <v>65193</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <v>175.2</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <f>C8*H8</f>
         <v>175.2</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" ht="211.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="11">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="8">
         <v>807</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <f>C10*H10</f>
         <v>3228</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="3"/>
+      <c r="K10" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
         <v>147.19999999999999</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="3">
         <f>C11*H11</f>
         <v>736</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>4</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3">
         <v>154.80799999999999</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <f>H12*C12</f>
         <v>619.23199999999997</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3">
         <v>203.2</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="3">
         <f>C14*H14</f>
         <v>203.2</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="3">
         <v>63197</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="3">
         <v>351.2</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="3">
         <f>C16*H16</f>
         <v>351.2</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>2</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="3">
         <v>433122</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3">
         <v>359.2</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="3">
         <f>C17*H17</f>
         <v>359.2</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="K17" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" ht="198" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="3">
         <v>60.14</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="3">
         <f t="shared" ref="I19:I24" si="0">C19*H19</f>
         <v>60.14</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6" t="s">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6" t="s">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="3">
         <v>4</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="3">
         <v>224.4</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="3">
         <f>C28*H28</f>
         <v>897.6</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6" t="s">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="3">
         <v>4</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="3">
         <v>198.352</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="3">
         <f>C29*H29</f>
         <v>793.40800000000002</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="3">
         <v>24</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="3">
         <v>309</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="3">
         <f>C30*H30</f>
         <v>7416</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K30" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="3">
         <v>10</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="3">
         <v>2536030320001</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="3">
         <v>0</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="3">
         <f>C32*H32</f>
         <v>0</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
     </row>
     <row r="34" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6">
+      <c r="G34" s="3"/>
+      <c r="H34" s="3">
         <v>698</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="3">
         <f>H34*C34</f>
         <v>698</v>
       </c>
-      <c r="J34" s="6"/>
-      <c r="K34" s="20" t="s">
+      <c r="J34" s="3"/>
+      <c r="K34" s="17" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="3">
         <v>1</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3">
         <v>349</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="3">
         <f>H35*C35</f>
         <v>349</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K35" s="20" t="s">
+      <c r="K35" s="17" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
+      <c r="A36" s="6">
         <v>2</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="3">
         <v>1</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="19">
         <v>41017348</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3">
         <v>199</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="3">
         <f t="shared" ref="I36" si="1">H36*C36</f>
         <v>199</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="8" t="s">
+      <c r="K36" s="5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="A37" s="7">
         <v>3</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="3">
         <v>1</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="3">
         <v>605.13</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="3">
         <f>C37*H37</f>
         <v>605.13</v>
       </c>
-      <c r="J37" s="6" t="s">
+      <c r="J37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K37" s="6" t="s">
+      <c r="K37" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-    </row>
-    <row r="39" spans="1:11" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+    </row>
+    <row r="39" spans="1:11" ht="79.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>1</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="3">
         <v>1</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="3">
         <v>2168</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6">
+      <c r="G39" s="3"/>
+      <c r="H39" s="3">
         <v>61</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="3">
         <f>H39*C39</f>
         <v>61</v>
       </c>
-      <c r="J39" s="6" t="s">
+      <c r="J39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K39" s="8" t="s">
+      <c r="K39" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="6">
-        <v>1</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="6">
+      <c r="E40" s="3">
         <v>2167</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6">
+      <c r="G40" s="3"/>
+      <c r="H40" s="3">
         <v>30.5</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="3">
         <f>H40*C40</f>
         <v>30.5</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="8"/>
+      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="3"/>
+      <c r="B42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="J42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K42" s="4" t="s">
+      <c r="K42" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="10"/>
+      <c r="B44" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="10"/>
+      <c r="B45" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="6" t="s">
+      <c r="A46" s="10"/>
+      <c r="B46" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="10"/>
+      <c r="B48" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="4" t="s">
+      <c r="A50" s="3"/>
+      <c r="B50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="G50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H50" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="3">
         <v>6</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7" t="s">
+      <c r="E52" s="3"/>
+      <c r="F52" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="G52" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H52" s="3">
         <v>262.83</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I52" s="3">
         <f>C52*H52</f>
         <v>1576.98</v>
       </c>
-      <c r="J52" s="6" t="s">
+      <c r="J52" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K52" s="6" t="s">
+      <c r="K52" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
-      <c r="B53" s="8" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C53" s="3">
         <v>1</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="3">
         <v>5901259432770</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G53" s="6" t="s">
+      <c r="G53" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H53" s="3">
         <v>237</v>
       </c>
-      <c r="I53" s="6">
+      <c r="I53" s="3">
         <f>C53*H53</f>
         <v>237</v>
       </c>
-      <c r="J53" s="6" t="s">
+      <c r="J53" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K53" s="6"/>
+      <c r="K53" s="3"/>
     </row>
     <row r="57" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C57" s="17">
+      <c r="C57" s="14">
         <f>SUM(I4,I11,I16,I19,I28,I37,I8)</f>
         <v>4013.2699999999995</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="18" t="s">
+      <c r="F57" s="22"/>
+      <c r="G57" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="6" t="s">
+      <c r="F58" s="2"/>
+      <c r="G58" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="9"/>
-      <c r="G59" s="6" t="s">
+      <c r="F59" s="6"/>
+      <c r="G59" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F60" s="10"/>
-      <c r="G60" s="6" t="s">
+      <c r="F60" s="7"/>
+      <c r="G60" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F61" s="13"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="3" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A31:K31"/>
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="A41:K41"/>
     <mergeCell ref="A49:K49"/>
     <mergeCell ref="A51:K51"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A13:K13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Updated a few of the links to the retailer website. One based on the feedback given by Henrik on preferred retailers and another since the previous was not up to date. I also added a sheet with the voltage levels specified in their respective datasheet for the primary component/sensor. By knowing all the voltage levels we can find out how many different voltage distribution circuits that need to be created as well as which component/sensor should be connected to which circuit.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_09976BEB9036F2153D1B5AD4644BDFF101C84B38" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D5C578D1-B026-49CB-9BC2-FF18964BB5C6}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_09976BEB9036F2153D1B5AD4644BDFF101C84B38" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2755CD21-8D60-4118-8AD5-F99662630425}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Voltage level" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="165">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -565,9 +566,6 @@
     <t>IR Break Beam 5mm LEDs</t>
   </si>
   <si>
-    <t>Adafruit 5mm</t>
-  </si>
-  <si>
     <t>Adafruit</t>
   </si>
   <si>
@@ -583,12 +581,63 @@
 have a greater diameter.
 These are sold at electro:kit</t>
   </si>
+  <si>
+    <t>Component/Sensor</t>
+  </si>
+  <si>
+    <t>Electro:kit - Adafruit 5mm</t>
+  </si>
+  <si>
+    <t>5901259432770</t>
+  </si>
+  <si>
+    <t>Voltage level 3.3</t>
+  </si>
+  <si>
+    <t>Voltage level 5.0</t>
+  </si>
+  <si>
+    <t>Voltage level 15V</t>
+  </si>
+  <si>
+    <t>Voltage level 24V</t>
+  </si>
+  <si>
+    <t>Voltage level 12V</t>
+  </si>
+  <si>
+    <t>x (continous)</t>
+  </si>
+  <si>
+    <t>x (intermittent)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x (preferred)</t>
+  </si>
+  <si>
+    <t>x (5.0V (±0.5))</t>
+  </si>
+  <si>
+    <t>x (DC 3.3V/0.5A)</t>
+  </si>
+  <si>
+    <t>x
+(DC 10V-44V 
+Since we have 24V
+that is most likely what we will use)</t>
+  </si>
+  <si>
+    <t>x (MAX 15V)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -666,6 +715,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -739,7 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -768,15 +822,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -975,39 +1036,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="71.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
-    <col min="5" max="5" width="35.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="115.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" customWidth="1"/>
-    <col min="11" max="11" width="40.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="118" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1045,19 +1106,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1158,19 +1219,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1207,19 +1268,19 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1314,19 +1375,19 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1359,19 +1420,19 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1442,19 +1503,19 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" ht="198" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1589,19 +1650,19 @@
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1639,19 +1700,19 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
@@ -1750,19 +1811,19 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1797,19 +1858,19 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
     </row>
     <row r="34" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -1948,19 +2009,19 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
     </row>
     <row r="39" spans="1:11" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
@@ -1973,13 +2034,13 @@
         <v>1</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E39" s="3">
         <v>2168</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3">
@@ -1993,25 +2054,25 @@
         <v>15</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="3">
         <v>2167</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3">
@@ -2027,19 +2088,19 @@
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
@@ -2096,7 +2157,7 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2175,19 +2236,19 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="21"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -2223,21 +2284,21 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+    </row>
+    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="3" t="s">
         <v>101</v>
@@ -2245,7 +2306,7 @@
       <c r="C52" s="3">
         <v>6</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="18" t="s">
         <v>53</v>
       </c>
       <c r="E52" s="3"/>
@@ -2280,8 +2341,8 @@
       <c r="D53" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="3">
-        <v>5901259432770</v>
+      <c r="E53" s="24" t="s">
+        <v>151</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>107</v>
@@ -2306,8 +2367,8 @@
         <v>109</v>
       </c>
       <c r="C57" s="14">
-        <f>SUM(I4,I11,I16,I19,I28,I37,I8)</f>
-        <v>4013.2699999999995</v>
+        <f>SUM(I4,I8,I16,I19,I28,I34,I39,I10)</f>
+        <v>6659.14</v>
       </c>
       <c r="E57" s="22" t="s">
         <v>110</v>
@@ -2404,22 +2465,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A31:K31"/>
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="A41:K41"/>
     <mergeCell ref="A49:K49"/>
     <mergeCell ref="A51:K51"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A13:K13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2464,4 +2525,123 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1084B6B2-930A-4914-817F-83AF4B9AD084}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>BOM!B52</f>
+        <v>LEDEX 195207-228</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>BOM!B39</f>
+        <v>IR Break Beam 5mm LEDs</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>BOM!B35</f>
+        <v>Raspberry Pi 3 model A+</v>
+      </c>
+      <c r="C4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>BOM!B32</f>
+        <v>WSEN-ISDS 6 Axis IMU</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>BOM!B28</f>
+        <v>iC-PX2604 + PX01S 26-30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>BOM!B14</f>
+        <v>ESP32-WROVER-IE</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>BOM!B10</f>
+        <v>Moetus R4</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>BOM!B4</f>
+        <v>Turnigy Multistar 4225-610Kv 16Pole Multi-Rotor Outrunner</v>
+      </c>
+      <c r="E9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the organisation of the excel files. Instead of having the voltage of the sensors as a sheet in BOM.xlsx I created a new excel file with the same information and put the file in Circuits/Voltage distribution directory.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_09976BEB9036F2153D1B5AD4644BDFF101C84B38" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2755CD21-8D60-4118-8AD5-F99662630425}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_09976BEB9036F2153D1B5AD4644BDFF101C84B38" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{019BEA3A-EB6D-4730-93F5-A78CF2265A21}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
-    <sheet name="Voltage level" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="151">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -582,62 +581,17 @@
 These are sold at electro:kit</t>
   </si>
   <si>
-    <t>Component/Sensor</t>
-  </si>
-  <si>
     <t>Electro:kit - Adafruit 5mm</t>
   </si>
   <si>
     <t>5901259432770</t>
-  </si>
-  <si>
-    <t>Voltage level 3.3</t>
-  </si>
-  <si>
-    <t>Voltage level 5.0</t>
-  </si>
-  <si>
-    <t>Voltage level 15V</t>
-  </si>
-  <si>
-    <t>Voltage level 24V</t>
-  </si>
-  <si>
-    <t>Voltage level 12V</t>
-  </si>
-  <si>
-    <t>x (continous)</t>
-  </si>
-  <si>
-    <t>x (intermittent)</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>x (preferred)</t>
-  </si>
-  <si>
-    <t>x (5.0V (±0.5))</t>
-  </si>
-  <si>
-    <t>x (DC 3.3V/0.5A)</t>
-  </si>
-  <si>
-    <t>x
-(DC 10V-44V 
-Since we have 24V
-that is most likely what we will use)</t>
-  </si>
-  <si>
-    <t>x (MAX 15V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -715,11 +669,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -793,7 +742,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -822,22 +771,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1036,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -1056,19 +1001,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1282,7 +1227,7 @@
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="1:11" ht="211.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="198" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
@@ -1650,19 +1595,19 @@
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -2009,21 +1954,21 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39" spans="1:11" ht="79.8" x14ac:dyDescent="0.3">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+    </row>
+    <row r="39" spans="1:11" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -2034,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E39" s="3">
         <v>2168</v>
@@ -2088,19 +2033,19 @@
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
@@ -2236,19 +2181,19 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -2341,8 +2286,8 @@
       <c r="D53" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="24" t="s">
-        <v>151</v>
+      <c r="E53" s="20" t="s">
+        <v>150</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>107</v>
@@ -2370,10 +2315,10 @@
         <f>SUM(I4,I8,I16,I19,I28,I34,I39,I10)</f>
         <v>6659.14</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="E57" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F57" s="22"/>
+      <c r="F57" s="23"/>
       <c r="G57" s="15" t="s">
         <v>111</v>
       </c>
@@ -2465,22 +2410,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A31:K31"/>
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="A41:K41"/>
     <mergeCell ref="A49:K49"/>
     <mergeCell ref="A51:K51"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A13:K13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2525,123 +2470,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1084B6B2-930A-4914-817F-83AF4B9AD084}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>BOM!B52</f>
-        <v>LEDEX 195207-228</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="D2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>BOM!B39</f>
-        <v>IR Break Beam 5mm LEDs</v>
-      </c>
-      <c r="B3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>BOM!B35</f>
-        <v>Raspberry Pi 3 model A+</v>
-      </c>
-      <c r="C4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>BOM!B32</f>
-        <v>WSEN-ISDS 6 Axis IMU</v>
-      </c>
-      <c r="B5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>BOM!B28</f>
-        <v>iC-PX2604 + PX01S 26-30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>BOM!B14</f>
-        <v>ESP32-WROVER-IE</v>
-      </c>
-      <c r="B7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>BOM!B10</f>
-        <v>Moetus R4</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>BOM!B4</f>
-        <v>Turnigy Multistar 4225-610Kv 16Pole Multi-Rotor Outrunner</v>
-      </c>
-      <c r="E9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the obsticle detection sensor section with up to date links and prices. Also promoted that the Raspberry Pi 4 Model B/8GB is the one we would like so that we can run both object detection as well as Nav2 on it.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3D5A4BCD5A37F2153DFB55874818ECB701B9D9ED" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{276DCEEF-4742-4A2A-8FEE-11F7D0DAF272}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_3D5A4BCD5A37F2153DFB55874818ECB701B9D9ED" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A8F71C2C-476C-48A3-AAB2-6ACD3178858E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="143">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t>IMU, Sponsored by W/E</t>
-  </si>
-  <si>
-    <t>Distance Sensors</t>
   </si>
   <si>
     <t>OPT8241NBN</t>
@@ -522,6 +519,39 @@
   </si>
   <si>
     <t>Voltage dividers (buck converters) -&gt; 15V</t>
+  </si>
+  <si>
+    <t>Already sent free of charge</t>
+  </si>
+  <si>
+    <t>Obsticle Detection Sensors</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Kameramodul 3</t>
+  </si>
+  <si>
+    <t>Electro:kit</t>
+  </si>
+  <si>
+    <t>41020240 - Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi 4 Model B/8GB </t>
+  </si>
+  <si>
+    <t>41017664 - Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4 Model B/4GB</t>
+  </si>
+  <si>
+    <t>41017110 - Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Secondary option</t>
   </si>
 </sst>
 </file>
@@ -679,17 +709,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -712,6 +733,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -908,1379 +939,1485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="71.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
-    <col min="5" max="5" width="35.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="115.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="118" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" customWidth="1"/>
-    <col min="11" max="11" width="40.33203125" customWidth="1"/>
+    <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>9392000008</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
         <v>297</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <f>C4*H4</f>
         <v>1188</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
         <v>215.4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <f>C5*H5</f>
         <v>861.6</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>54896</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="11">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="8">
         <v>268.8</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <f>C6*H6</f>
         <v>1075.2</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <v>65193</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <v>175.2</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <f>C8*H8</f>
         <v>175.2</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="211.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="11">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="8">
         <v>807</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <f>C10*H10</f>
         <v>3228</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="3"/>
+      <c r="K10" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
         <v>147.19999999999999</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="3">
         <f>C11*H11</f>
         <v>736</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>4</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3">
         <v>154.80799999999999</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <f>H12*C12</f>
         <v>619.23199999999997</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3">
         <v>203.2</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="3">
         <f>C14*H14</f>
         <v>203.2</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="3">
         <v>63197</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="3">
         <v>351.2</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="3">
         <f>C16*H16</f>
         <v>351.2</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>2</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="3">
         <v>433122</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3">
         <v>359.2</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="3">
         <f>C17*H17</f>
         <v>359.2</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="K17" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="198" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="3">
         <v>146.92500000000001</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="3">
         <f t="shared" ref="I19:I24" si="0">C19*H19</f>
         <v>146.92500000000001</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6" t="s">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6" t="s">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="3">
         <v>4</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="3">
         <v>224.4</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="3">
         <f>C28*H28</f>
         <v>897.6</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6" t="s">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="3">
         <v>4</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="3">
         <v>198.352</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="3">
         <f>C29*H29</f>
         <v>793.40800000000002</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="3">
         <v>24</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="3">
         <v>309</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="3">
         <f>C30*H30</f>
         <v>7416</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K30" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="3">
         <v>10</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7" t="s">
+      <c r="D32" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="3">
         <v>2536030320001</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="3">
         <v>0</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="3">
         <f>C32*H32</f>
         <v>0</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3">
+        <v>369</v>
+      </c>
+      <c r="I34" s="3">
+        <f>H34*C34</f>
+        <v>369</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="22" t="str">
+        <f>"Needs to be ordered with " &amp; BOM!B35</f>
+        <v xml:space="preserve">Needs to be ordered with Raspberry Pi 4 Model B/8GB </v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3">
+        <v>979</v>
+      </c>
+      <c r="I35" s="3">
+        <f>H35*C35</f>
+        <v>979</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="3" t="str">
+        <f>"Can be substituted with " &amp; BOM!B36</f>
+        <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3">
+        <v>729</v>
+      </c>
+      <c r="I36" s="3">
+        <f>H36*C36</f>
+        <v>729</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6" t="s">
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="6">
+      <c r="F37" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="3">
+        <v>605.13</v>
+      </c>
+      <c r="I37" s="3">
+        <f>C37*H37</f>
+        <v>605.13</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E46" s="18">
+        <v>173010335</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="3">
+        <v>3</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" s="18">
+        <v>173010542</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" s="3">
+        <v>173011235</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="3">
+        <v>3</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E49" s="18">
+        <v>173011535</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="3">
+        <v>6</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="3">
+        <v>262.83</v>
+      </c>
+      <c r="I53" s="3">
+        <f>C53*H53</f>
+        <v>1576.98</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H34" s="6">
-        <v>605.13</v>
-      </c>
-      <c r="I34" s="6">
-        <f>C34*H34</f>
-        <v>605.13</v>
-      </c>
-      <c r="J34" s="6" t="s">
+      <c r="D54" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="3">
+        <v>5901259432770</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H54" s="3">
+        <v>237</v>
+      </c>
+      <c r="I54" s="3">
+        <f>C54*H54</f>
+        <v>237</v>
+      </c>
+      <c r="J54" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
-      <c r="B43" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="6">
-        <v>3</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="E43" s="21">
-        <v>173010335</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6">
-        <v>0</v>
-      </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K43" s="6"/>
-    </row>
-    <row r="44" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C44" s="6">
-        <v>3</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="21">
-        <v>173010542</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6">
-        <v>0</v>
-      </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K44" s="6"/>
-    </row>
-    <row r="45" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C45" s="6">
-        <v>3</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="6">
-        <v>173011235</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6">
-        <v>0</v>
-      </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" s="6"/>
-    </row>
-    <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="6">
-        <v>3</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="E46" s="21">
-        <v>173011535</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6">
-        <v>0</v>
-      </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K46" s="6"/>
-    </row>
-    <row r="47" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="K54" s="3"/>
+    </row>
+    <row r="58" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B58" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="14">
+        <f>SUM(I4,I11,I16,I19,I28,I8,I34,I35)</f>
+        <v>4842.9249999999993</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="21"/>
+      <c r="G58" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B59" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F60" s="6"/>
+      <c r="G60" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" s="6">
-        <v>6</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H50" s="6">
-        <v>262.83</v>
-      </c>
-      <c r="I50" s="6">
-        <f>C50*H50</f>
-        <v>1576.98</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K50" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="6">
-        <v>1</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E51" s="6">
-        <v>5901259432770</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H51" s="6">
-        <v>237</v>
-      </c>
-      <c r="I51" s="6">
-        <f>C51*H51</f>
-        <v>237</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K51" s="6"/>
-    </row>
-    <row r="55" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B55" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C55" s="17">
-        <f>SUM(I4,I11,I16,I19,I28,I34,I8)</f>
-        <v>4100.0550000000003</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B56" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B57" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="6" t="s">
+      <c r="E61" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E58" s="6" t="s">
+      <c r="F61" s="7"/>
+      <c r="G61" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F58" s="10"/>
-      <c r="G58" s="6" t="s">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E59" s="6" t="s">
+      <c r="F62" s="10"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F59" s="13"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="6" t="s">
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="6" t="s">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="6" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="6" t="s">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A13:K13"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A18:K18"/>
     <mergeCell ref="A25:K25"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="E58:F58"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2306,19 +2443,22 @@
     <hyperlink ref="F30" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="D32" r:id="rId22" display="Würth Electronik" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="F32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D34" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D50" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F50" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D51" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="F51" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D43" r:id="rId30" xr:uid="{352F57A6-E97F-43AC-9712-9812F7A1FE21}"/>
-    <hyperlink ref="D44" r:id="rId31" xr:uid="{63700873-F78F-4675-9A1A-C886902A23FB}"/>
-    <hyperlink ref="D45" r:id="rId32" xr:uid="{7F06459F-E31F-43B8-B9BD-5E6BD0072056}"/>
-    <hyperlink ref="D46" r:id="rId33" xr:uid="{499E06DB-AA6B-4B38-9FCB-35249B741E10}"/>
+    <hyperlink ref="D37" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F37" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D53" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F53" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D54" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F54" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D46" r:id="rId30" xr:uid="{352F57A6-E97F-43AC-9712-9812F7A1FE21}"/>
+    <hyperlink ref="D47" r:id="rId31" xr:uid="{63700873-F78F-4675-9A1A-C886902A23FB}"/>
+    <hyperlink ref="D48" r:id="rId32" xr:uid="{7F06459F-E31F-43B8-B9BD-5E6BD0072056}"/>
+    <hyperlink ref="D49" r:id="rId33" xr:uid="{499E06DB-AA6B-4B38-9FCB-35249B741E10}"/>
+    <hyperlink ref="D35" r:id="rId34" xr:uid="{95461AE4-C8EA-491B-8B80-A8FE4949F22E}"/>
+    <hyperlink ref="D34" r:id="rId35" xr:uid="{5926EC95-A3F8-46AB-991F-3BB51A67B78E}"/>
+    <hyperlink ref="D36" r:id="rId36" xr:uid="{B15B4C47-2C00-4A79-9B58-85B797E723ED}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId37"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Changed the colour classification of the obsticle sensors.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\SSL-Hardware-Development\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_3D5A4BCD5A37F2153DFB55874818ECB701B9D9ED" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A8F71C2C-476C-48A3-AAB2-6ACD3178858E}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_3D5A4BCD5A37F2153DFB55874818ECB701B9D9ED" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3093BB83-C518-42E5-AEE8-15962A556B0D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,16 +733,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1011,19 +1011,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1124,19 +1124,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1173,21 +1173,21 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" ht="211.2" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
@@ -1280,19 +1280,19 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1325,19 +1325,19 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1408,19 +1408,19 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" ht="198" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1605,19 +1605,19 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
@@ -1716,19 +1716,19 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1763,19 +1763,19 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1805,7 +1805,7 @@
       <c r="J34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="22" t="str">
+      <c r="K34" s="19" t="str">
         <f>"Needs to be ordered with " &amp; BOM!B35</f>
         <v xml:space="preserve">Needs to be ordered with Raspberry Pi 4 Model B/8GB </v>
       </c>
@@ -1844,7 +1844,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="3" t="s">
         <v>140</v>
       </c>
@@ -1876,7 +1876,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -2222,19 +2222,19 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -2308,10 +2308,10 @@
         <f>SUM(I4,I11,I16,I19,I28,I8,I34,I35)</f>
         <v>4842.9249999999993</v>
       </c>
-      <c r="E58" s="21" t="s">
+      <c r="E58" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F58" s="21"/>
+      <c r="F58" s="22"/>
       <c r="G58" s="15" t="s">
         <v>111</v>
       </c>
@@ -2403,21 +2403,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A31:K31"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A7:K7"/>
     <mergeCell ref="A9:K9"/>
     <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A50:K50"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="E58:F58"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Made some minor changes to the BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_A40B5F03F119087C648284DB62138A0AD4CFEFE7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B99A1A23-65A0-4756-B7B3-9D662AB1D97B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_A40B5F03F119087C648284DB62138A0AD4CFEFE7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{069A2705-9571-4E5B-8F1E-EB623579B341}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="149">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -671,6 +671,9 @@
   </si>
   <si>
     <t>Temperature sensors</t>
+  </si>
+  <si>
+    <t>Passive components</t>
   </si>
 </sst>
 </file>
@@ -853,17 +856,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -883,13 +877,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -907,6 +899,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1103,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1125,1497 +1126,1527 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" spans="1:11" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4">
         <v>818.4</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="4">
         <f>C4*H4</f>
         <v>3273.6</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="25">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>4</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="8">
         <v>9392000008</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8">
         <v>297</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="8">
         <f>C5*H5</f>
         <v>1188</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8">
         <v>215.4</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="8">
         <f>C6*H6</f>
         <v>861.6</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="19">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>4</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="8">
         <v>54896</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="16">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="11">
         <v>268.8</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="8">
         <f>C7*H7</f>
         <v>1075.2</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="8">
         <v>1</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="8">
         <v>65193</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="8">
         <v>175.2</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="8">
         <f>C9*H9</f>
         <v>175.2</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="13">
         <v>1</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="8">
         <v>4</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="16">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="11">
         <v>807</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="8">
         <f>C11*H11</f>
         <v>3228</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="14" t="s">
+      <c r="J11" s="8"/>
+      <c r="K11" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="25">
         <v>2</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="8">
         <v>5</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8">
         <v>147.19999999999999</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="8">
         <f>C12*H12</f>
         <v>736</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
+      <c r="A13" s="19">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="8">
         <v>4</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8">
         <v>154.80799999999999</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="8">
         <f>H13*C13</f>
         <v>619.23199999999997</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="12">
         <v>1</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="8">
         <v>1</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8">
         <v>203.2</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="8">
         <f>C15*H15</f>
         <v>203.2</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="A16" s="12">
         <v>1</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8">
         <v>979</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="8">
         <f>H16*C16</f>
         <v>979</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="12" t="str">
+      <c r="K16" s="8" t="str">
         <f>"Can be substituted with " &amp; BOM!B17</f>
         <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12">
+      <c r="G17" s="8"/>
+      <c r="H17" s="8">
         <v>729</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="8">
         <f>H17*C17</f>
         <v>729</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="A19" s="12">
         <v>1</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="8">
         <v>1</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="8">
         <v>63197</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="8">
         <v>351.2</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="8">
         <f>C19*H19</f>
         <v>351.2</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="A20" s="25">
         <v>2</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="8">
         <v>1</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="8">
         <v>433122</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12">
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8">
         <v>359.2</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="8">
         <f>C20*H20</f>
         <v>359.2</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11" ht="184.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="A22" s="12">
         <v>1</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="8">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="8">
         <v>146.92500000000001</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="8">
         <f t="shared" ref="I22:I27" si="0">C22*H22</f>
         <v>146.92500000000001</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12" t="s">
+      <c r="J23" s="8"/>
+      <c r="K23" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="12" t="s">
+      <c r="A24" s="16"/>
+      <c r="B24" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12" t="s">
+      <c r="J24" s="8"/>
+      <c r="K24" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="12" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12" t="s">
+      <c r="J25" s="8"/>
+      <c r="K25" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
     </row>
     <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="12" t="s">
+      <c r="A31" s="12"/>
+      <c r="B31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="8">
         <v>4</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="22" t="s">
+      <c r="E31" s="15"/>
+      <c r="F31" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="8">
         <v>224.4</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="8">
         <f>C31*H31</f>
         <v>897.6</v>
       </c>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12" t="s">
+      <c r="J31" s="8"/>
+      <c r="K31" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="8">
         <v>4</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="8">
         <v>198.352</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="8">
         <f>C32*H32</f>
         <v>793.40800000000002</v>
       </c>
-      <c r="J32" s="12" t="s">
+      <c r="J32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="K32" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="8">
         <v>24</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13" t="s">
+      <c r="E33" s="8"/>
+      <c r="F33" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="8">
         <v>309</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="8">
         <f>C33*H33</f>
         <v>7416</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="K33" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="8">
         <v>10</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13" t="s">
+      <c r="E35" s="8"/>
+      <c r="F35" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="8">
         <v>2536030320001</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="8">
         <v>0</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="8">
         <f>C35*H35</f>
         <v>0</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="12" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="8">
         <v>1</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12">
+      <c r="G37" s="8"/>
+      <c r="H37" s="8">
         <v>369</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="8">
         <f>H37*C37</f>
         <v>369</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="J37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K37" s="23" t="str">
+      <c r="K37" s="18" t="str">
         <f>"Needs to be ordered with " &amp; BOM!B16 &amp; "or " &amp; BOM!B17</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="8">
         <v>1</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G38" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38" s="8">
         <v>605.13</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38" s="8">
         <f>C38*H38</f>
         <v>605.13</v>
       </c>
-      <c r="J38" s="12" t="s">
+      <c r="J38" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="12" t="s">
+      <c r="K38" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="12" t="s">
+    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="B42" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="12" t="s">
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="B43" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12" t="s">
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="12" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12" t="s">
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="12" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
+      <c r="B45" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12" t="s">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="12" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+      <c r="B46" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12" t="s">
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="12" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12" t="s">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="21"/>
-      <c r="B47" s="12" t="s">
+    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+    </row>
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="16"/>
+      <c r="B49" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C49" s="8">
         <v>3</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D49" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E49" s="20">
         <v>173010335</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F49" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12">
+      <c r="G49" s="8"/>
+      <c r="H49" s="8">
         <v>0</v>
       </c>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12" t="s">
+      <c r="I49" s="8"/>
+      <c r="J49" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="K49" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
-      <c r="B48" s="12" t="s">
+    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="16"/>
+      <c r="B50" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C50" s="8">
         <v>3</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D50" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E50" s="20">
         <v>173010542</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F50" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12">
+      <c r="G50" s="8"/>
+      <c r="H50" s="8">
         <v>0</v>
       </c>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12" t="s">
+      <c r="I50" s="8"/>
+      <c r="J50" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="K50" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="12" t="s">
+    <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="16"/>
+      <c r="B51" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C51" s="8">
         <v>3</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D51" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="12">
+      <c r="E51" s="8">
         <v>173011235</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F51" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12">
+      <c r="G51" s="8"/>
+      <c r="H51" s="8">
         <v>0</v>
       </c>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12" t="s">
+      <c r="I51" s="8"/>
+      <c r="J51" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="K51" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="12" t="s">
+    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="16"/>
+      <c r="B52" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C52" s="8">
         <v>3</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D52" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E52" s="20">
         <v>173011535</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F52" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12">
+      <c r="G52" s="8"/>
+      <c r="H52" s="8">
         <v>0</v>
       </c>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12" t="s">
+      <c r="I52" s="8"/>
+      <c r="J52" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="K52" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="53" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="H54" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="I54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="J54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="K54" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A55" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="12" t="s">
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="12">
+      <c r="C56" s="8">
         <v>6</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D56" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="13" t="s">
+      <c r="E56" s="8"/>
+      <c r="F56" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G56" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="H54" s="12">
+      <c r="H56" s="8">
         <v>262.83</v>
       </c>
-      <c r="I54" s="12">
-        <f>C54*H54</f>
+      <c r="I56" s="8">
+        <f>C56*H56</f>
         <v>1576.98</v>
       </c>
-      <c r="J54" s="12" t="s">
+      <c r="J56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K54" s="12" t="s">
+      <c r="K56" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="14" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="25"/>
+      <c r="B57" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="12">
+      <c r="C57" s="8">
         <v>1</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D57" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E55" s="12">
+      <c r="E57" s="8">
         <v>5901259432770</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F57" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="G55" s="12" t="s">
+      <c r="G57" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H55" s="12">
+      <c r="H57" s="8">
         <v>237</v>
       </c>
-      <c r="I55" s="12">
-        <f>C55*H55</f>
+      <c r="I57" s="8">
+        <f>C57*H57</f>
         <v>237</v>
       </c>
-      <c r="J55" s="12" t="s">
+      <c r="J57" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K55" s="12"/>
-    </row>
-    <row r="59" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B59" s="26" t="s">
+      <c r="K57" s="8"/>
+    </row>
+    <row r="61" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B61" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C59" s="27" t="e">
+      <c r="C61" s="22" t="e">
         <f>SUM(I5,I12,I19,I22,I31,I9,I37,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E61" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="28" t="s">
+      <c r="F61" s="28"/>
+      <c r="G61" s="23" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B60" s="29" t="s">
+    <row r="62" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B62" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E62" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F60" s="17"/>
-      <c r="G60" s="12" t="s">
+      <c r="F62" s="12"/>
+      <c r="G62" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B61" s="12" t="s">
+    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E63" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F61" s="30"/>
-      <c r="G61" s="12" t="s">
+      <c r="F63" s="25"/>
+      <c r="G63" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E64" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F62" s="24"/>
-      <c r="G62" s="12" t="s">
+      <c r="F64" s="19"/>
+      <c r="G64" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="12" t="s">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E65" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F63" s="21"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="12" t="s">
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="12" t="s">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="12" t="s">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="12" t="s">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="12" t="s">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="12" t="s">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="12" t="s">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="E59:F59"/>
+  <mergeCells count="17">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A18:K18"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A30:K30"/>
     <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A48:K48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2647,14 +2678,14 @@
     <hyperlink ref="D37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="D38" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="F38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D48" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D54" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F54" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D55" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F55" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D49" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D50" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D51" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D52" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D56" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F56" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D57" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F57" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added the break beam sensor that has been lost. I also included comments to the prices that I know include moms.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_A40B5F03F119087C648284DB62138A0AD4CFEFE7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{069A2705-9571-4E5B-8F1E-EB623579B341}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_A40B5F03F119087C648284DB62138A0AD4CFEFE7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{EF450F3F-8B33-464F-822B-0369F5C09891}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Fredrik Westerbom</author>
+  </authors>
+  <commentList>
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{9644850F-A885-4263-859B-12A408B91E84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fredrik Westerbom:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Incl. moms</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{4C444A5F-4FBA-4135-ACF9-D91835DC1602}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fredrik Westerbom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Incl. Moms</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="0" shapeId="0" xr:uid="{6953005F-94C6-472F-BCFA-4E16CE6F3AA7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fredrik Westerbom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Incl. moms</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H40" authorId="0" shapeId="0" xr:uid="{ACFBBAF4-03FE-4DC5-8BD3-23F36BEB7970}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fredrik Westerbom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Incl. moms</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="153">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -389,9 +495,6 @@
   </si>
   <si>
     <t xml:space="preserve">OPT8241NBN </t>
-  </si>
-  <si>
-    <t>Brake beam, Distance sensor</t>
   </si>
   <si>
     <t>3D CAD and Mechanical</t>
@@ -675,12 +778,27 @@
   <si>
     <t>Passive components</t>
   </si>
+  <si>
+    <t>Break Beam sensor</t>
+  </si>
+  <si>
+    <t>IR Break Beam Sensor - 5mm LEDs</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Distance sensor</t>
+  </si>
+  <si>
+    <t>Break beam to detect if a ball is close (within a few mm) to the dribbler.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -783,6 +901,32 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -856,7 +1000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -882,7 +1026,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -895,19 +1038,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1103,11 +1254,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1119,26 +1270,26 @@
     <col min="5" max="5" width="22.5546875" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="118" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="8" style="32" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="32" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
     <col min="11" max="11" width="99.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1162,10 +1313,10 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="28" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -1176,19 +1327,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1208,10 +1359,10 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="4">
+      <c r="H4" s="29">
         <v>818.4</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="29">
         <f>C4*H4</f>
         <v>3273.6</v>
       </c>
@@ -1223,7 +1374,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1240,10 +1391,10 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="H5" s="30">
         <v>297</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="30">
         <f>C5*H5</f>
         <v>1188</v>
       </c>
@@ -1255,7 +1406,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1274,10 +1425,10 @@
         <v>25</v>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="8">
+      <c r="H6" s="30">
         <v>215.4</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="30">
         <f>C6*H6</f>
         <v>861.6</v>
       </c>
@@ -1289,7 +1440,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1306,10 +1457,10 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="11">
+      <c r="H7" s="31">
         <v>268.8</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="30">
         <f>C7*H7</f>
         <v>1075.2</v>
       </c>
@@ -1321,22 +1472,22 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
@@ -1355,10 +1506,10 @@
       <c r="G9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="30">
         <v>175.2</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="30">
         <f>C9*H9</f>
         <v>175.2</v>
       </c>
@@ -1370,22 +1521,22 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>1</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1400,10 +1551,10 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="11">
+      <c r="H11" s="31">
         <v>807</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="30">
         <f>C11*H11</f>
         <v>3228</v>
       </c>
@@ -1413,7 +1564,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="25">
+      <c r="A12" s="23">
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1430,10 +1581,10 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8">
+      <c r="H12" s="30">
         <v>147.19999999999999</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="30">
         <f>C12*H12</f>
         <v>736</v>
       </c>
@@ -1445,7 +1596,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1462,10 +1613,10 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="8">
+      <c r="H13" s="30">
         <v>154.80799999999999</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="30">
         <f>H13*C13</f>
         <v>619.23199999999997</v>
       </c>
@@ -1477,22 +1628,22 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <v>1</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1507,10 +1658,10 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="8">
+      <c r="H15" s="30">
         <v>203.2</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="30">
         <f>C15*H15</f>
         <v>203.2</v>
       </c>
@@ -1522,7 +1673,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <v>1</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1531,7 +1682,7 @@
       <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1541,10 +1692,10 @@
         <v>53</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="8">
+      <c r="H16" s="30">
         <v>979</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="30">
         <f>H16*C16</f>
         <v>979</v>
       </c>
@@ -1557,14 +1708,14 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="8" t="s">
@@ -1574,10 +1725,10 @@
         <v>53</v>
       </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="8">
+      <c r="H17" s="30">
         <v>729</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="30">
         <f>H17*C17</f>
         <v>729</v>
       </c>
@@ -1589,22 +1740,22 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="11">
         <v>1</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1625,10 +1776,10 @@
       <c r="G19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="30">
         <v>351.2</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="30">
         <f>C19*H19</f>
         <v>351.2</v>
       </c>
@@ -1640,7 +1791,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="25">
+      <c r="A20" s="23">
         <v>2</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1657,10 +1808,10 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="8">
+      <c r="H20" s="30">
         <v>359.2</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="30">
         <f>C20*H20</f>
         <v>359.2</v>
       </c>
@@ -1672,22 +1823,22 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
     </row>
     <row r="22" spans="1:11" ht="184.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="11">
         <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -1708,10 +1859,10 @@
       <c r="G22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="30">
         <v>146.92500000000001</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="30">
         <f t="shared" ref="I22:I27" si="0">C22*H22</f>
         <v>146.92500000000001</v>
       </c>
@@ -1723,7 +1874,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>70</v>
       </c>
@@ -1732,8 +1883,8 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8">
+      <c r="H23" s="30"/>
+      <c r="I23" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1743,7 +1894,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="8" t="s">
         <v>72</v>
       </c>
@@ -1752,8 +1903,8 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8">
+      <c r="H24" s="30"/>
+      <c r="I24" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1763,7 +1914,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="8" t="s">
         <v>73</v>
       </c>
@@ -1772,8 +1923,8 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8">
+      <c r="H25" s="30"/>
+      <c r="I25" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1783,7 +1934,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="8" t="s">
         <v>74</v>
       </c>
@@ -1792,8 +1943,8 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8">
+      <c r="H26" s="30"/>
+      <c r="I26" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1801,7 +1952,7 @@
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="8" t="s">
         <v>75</v>
       </c>
@@ -1810,8 +1961,8 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8">
+      <c r="H27" s="30"/>
+      <c r="I27" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1819,19 +1970,19 @@
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1855,10 +2006,10 @@
       <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="28" t="s">
         <v>9</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -1869,42 +2020,42 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C31" s="8">
         <v>4</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="17" t="s">
+      <c r="E31" s="14"/>
+      <c r="F31" s="16" t="s">
         <v>80</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="30">
         <v>224.4</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="30">
         <f>C31*H31</f>
         <v>897.6</v>
       </c>
@@ -1914,7 +2065,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="8" t="s">
         <v>83</v>
       </c>
@@ -1933,10 +2084,10 @@
       <c r="G32" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="30">
         <v>198.352</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="30">
         <f>C32*H32</f>
         <v>793.40800000000002</v>
       </c>
@@ -1948,7 +2099,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="8" t="s">
         <v>88</v>
       </c>
@@ -1965,10 +2116,10 @@
       <c r="G33" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="30">
         <v>309</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="30">
         <f>C33*H33</f>
         <v>7416</v>
       </c>
@@ -1980,22 +2131,22 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="8" t="s">
         <v>95</v>
       </c>
@@ -2012,10 +2163,10 @@
       <c r="G35" s="8">
         <v>2536030320001</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="30">
         <v>0</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="30">
         <f>C35*H35</f>
         <v>0</v>
       </c>
@@ -2027,29 +2178,29 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="13" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="8" t="s">
@@ -2059,23 +2210,23 @@
         <v>53</v>
       </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="8">
+      <c r="H37" s="30">
         <v>369</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="30">
         <f>H37*C37</f>
         <v>369</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K37" s="18" t="str">
+      <c r="K37" s="17" t="str">
         <f>"Needs to be ordered with " &amp; BOM!B16 &amp; "or " &amp; BOM!B17</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="8" t="s">
         <v>102</v>
       </c>
@@ -2088,16 +2239,16 @@
       <c r="E38" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>104</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="30">
         <v>605.13</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="30">
         <f>C38*H38</f>
         <v>605.13</v>
       </c>
@@ -2105,548 +2256,596 @@
         <v>20</v>
       </c>
       <c r="K38" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+    </row>
+    <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+      <c r="B40" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="8">
+        <v>1</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="8">
+        <v>41015028</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="30">
+        <v>99</v>
+      </c>
+      <c r="I40" s="30">
+        <f>H40*C40</f>
+        <v>99</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="8" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-    </row>
-    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
       <c r="B49" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="8">
-        <v>3</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="20">
-        <v>173010335</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>97</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="8">
-        <v>0</v>
-      </c>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="8"/>
       <c r="K49" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="8">
-        <v>3</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="20">
-        <v>173010542</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8">
-        <v>0</v>
-      </c>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K50" s="8" t="s">
-        <v>116</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
     </row>
     <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="16"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C51" s="8">
         <v>3</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="8">
-        <v>173011235</v>
+      <c r="E51" s="19">
+        <v>173010335</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>97</v>
       </c>
       <c r="G51" s="8"/>
-      <c r="H51" s="8">
+      <c r="H51" s="30">
         <v>0</v>
       </c>
-      <c r="I51" s="8"/>
+      <c r="I51" s="30"/>
       <c r="J51" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K51" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="15"/>
+      <c r="B52" s="8" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="C52" s="8">
         <v>3</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="20">
-        <v>173011535</v>
+      <c r="E52" s="19">
+        <v>173010542</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>97</v>
       </c>
       <c r="G52" s="8"/>
-      <c r="H52" s="8">
+      <c r="H52" s="30">
         <v>0</v>
       </c>
-      <c r="I52" s="8"/>
+      <c r="I52" s="30"/>
       <c r="J52" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="15"/>
+      <c r="B53" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="8">
+        <v>3</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="8">
+        <v>173011235</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="H53" s="30">
+        <v>0</v>
+      </c>
+      <c r="I53" s="30"/>
+      <c r="J53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="15"/>
+      <c r="B54" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="8">
+        <v>3</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="19">
+        <v>173011535</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="H54" s="30">
+        <v>0</v>
+      </c>
+      <c r="I54" s="30"/>
+      <c r="J54" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="24"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I56" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A57" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="1" t="s">
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="25"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="8">
         <v>6</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="8" t="s">
+      <c r="D58" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="8">
-        <v>6</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E56" s="8"/>
-      <c r="F56" s="9" t="s">
+      <c r="G58" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="H58" s="30">
+        <v>262.83</v>
+      </c>
+      <c r="I58" s="30">
+        <f>C58*H58</f>
+        <v>1576.98</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="H56" s="8">
-        <v>262.83</v>
-      </c>
-      <c r="I56" s="8">
-        <f>C56*H56</f>
-        <v>1576.98</v>
-      </c>
-      <c r="J56" s="8" t="s">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="8">
+        <v>1</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E59" s="8">
+        <v>5901259432770</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H59" s="30">
+        <v>237</v>
+      </c>
+      <c r="I59" s="30">
+        <f>C59*H59</f>
+        <v>237</v>
+      </c>
+      <c r="J59" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K56" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
-      <c r="B57" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" s="8">
-        <v>1</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E57" s="8">
-        <v>5901259432770</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G57" s="8" t="s">
+      <c r="K59" s="8"/>
+    </row>
+    <row r="63" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B63" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="H57" s="8">
-        <v>237</v>
-      </c>
-      <c r="I57" s="8">
-        <f>C57*H57</f>
-        <v>237</v>
-      </c>
-      <c r="J57" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K57" s="8"/>
-    </row>
-    <row r="61" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B61" s="21" t="s">
+      <c r="C63" s="27">
+        <f>SUM(I4,I11,I19,I22,I31,I9,I37,I58)</f>
+        <v>10018.505000000001</v>
+      </c>
+      <c r="E63" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="22" t="e">
-        <f>SUM(I5,I12,I19,I22,I31,I9,I37,#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E61" s="28" t="s">
+      <c r="F63" s="26"/>
+      <c r="G63" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F61" s="28"/>
-      <c r="G61" s="23" t="s">
+    </row>
+    <row r="64" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B64" s="22" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B62" s="24" t="s">
+      <c r="E64" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="F64" s="11"/>
+      <c r="G64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F62" s="12"/>
-      <c r="G62" s="8" t="s">
+    </row>
+    <row r="65" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B63" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="F65" s="23"/>
+      <c r="G65" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F63" s="25"/>
-      <c r="G63" s="8" t="s">
+    </row>
+    <row r="66" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B64" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E64" s="8" t="s">
+      <c r="F66" s="18"/>
+      <c r="G66" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F64" s="19"/>
-      <c r="G64" s="8" t="s">
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" s="8" t="s">
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F65" s="16"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="8" t="s">
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="8" t="s">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="8" t="s">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="8" t="s">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="8" t="s">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="8" t="s">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A34:K34"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="A14:K14"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A28:K28"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A55:K55"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A48:K48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2678,20 +2877,22 @@
     <hyperlink ref="D37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="D38" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="F38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D49" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D50" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D51" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D52" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D56" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F56" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D57" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F57" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D51" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D52" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D53" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D54" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D58" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F58" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D59" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F59" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D40" r:id="rId38" xr:uid="{2D087B20-628E-4347-A76D-7D74376AF2B9}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId39"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added alternative motor driver B-G431B-ESC1, Nucleo 144 Dev board as alternative to ESP32, RF tranceivers that are proven to be reliable for communication with server laptop
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -25,7 +25,7 @@
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="H17" authorId="0">
+    <comment ref="H18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0">
+    <comment ref="H20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H38" authorId="0">
+    <comment ref="H43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H41" authorId="0">
+    <comment ref="H46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="175">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -273,6 +273,18 @@
     <t xml:space="preserve">N-Channel mosfet drivers for the BLDC motors</t>
   </si>
   <si>
+    <t xml:space="preserve">B-G431B-ESC1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-B-G431B-ESC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMicroelectronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datasheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aerostar 30A RVS G2 32bit ESC</t>
   </si>
   <si>
@@ -318,6 +330,16 @@
     <t xml:space="preserve">Raspberry Pi</t>
   </si>
   <si>
+    <t xml:space="preserve">NUCLEO-H723ZG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-NUCLEO-H723ZG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If we do not develop our own pcb this microcontroller can be used instead of the ESP32 microcontroll-
+Er, ADC, communication, supports micro ros</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raspberry Pi 4 Model B/4GB</t>
   </si>
   <si>
@@ -325,6 +347,36 @@
   </si>
   <si>
     <t xml:space="preserve">Secondary option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF (Radio frequency)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SX1280IMLTRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">947-SX1280IMLTRT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semtech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF Transceiver Long range 2.4 GHz Wireless Transceiver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKY66122-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">873-SKY66122-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skyworks Solutions, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKY66122-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF Front End OFDM, 863 to 928 MHz, Wi-SUN, FEM</t>
   </si>
   <si>
     <t xml:space="preserve">Battery</t>
@@ -650,9 +702,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">We will not be able to test the SMD sensors, we will need a circuit for that first. Alternatively find a THT component replacement for developing</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -681,9 +730,6 @@
       </rPr>
       <t xml:space="preserve"> choice</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">We need motors + escs to start developing the driving interface</t>
   </si>
   <si>
     <t xml:space="preserve">Might need</t>
@@ -774,6 +820,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
@@ -786,13 +839,6 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -927,11 +973,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1024,7 +1070,39 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1032,15 +1110,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1252,25 +1326,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="118"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="99.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="71.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="81.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,705 +1674,725 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+    <row r="13" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="B13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="9" t="n">
+        <v>208.96</v>
+      </c>
+      <c r="I13" s="9" t="n">
+        <f aca="false">C13*H13</f>
+        <v>1044.8</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="n">
         <v>2</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="17" t="n">
-        <v>147.2</v>
-      </c>
-      <c r="I13" s="17" t="n">
-        <f aca="false">C13*H13</f>
-        <v>736</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="n">
-        <v>3</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="17" t="n">
-        <v>154.808</v>
+        <v>147.2</v>
       </c>
       <c r="I14" s="17" t="n">
-        <f aca="false">H14*C14</f>
-        <v>619.232</v>
+        <f aca="false">C14*H14</f>
+        <v>736</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="K14" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="15" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="C15" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17" t="n">
-        <v>203.2</v>
-      </c>
-      <c r="I16" s="17" t="n">
-        <f aca="false">C16*H16</f>
-        <v>203.2</v>
-      </c>
-      <c r="J16" s="15" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="17" t="n">
+        <v>154.808</v>
+      </c>
+      <c r="I15" s="17" t="n">
+        <f aca="false">H15*C15</f>
+        <v>619.232</v>
+      </c>
+      <c r="J15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="K15" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="15" t="s">
         <v>61</v>
       </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="17" t="n">
-        <v>979</v>
+        <v>203.2</v>
       </c>
       <c r="I17" s="17" t="n">
-        <f aca="false">H17*C17</f>
-        <v>979</v>
+        <f aca="false">C17*H17</f>
+        <v>203.2</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="15" t="str">
-        <f aca="false">"Can be substituted with " &amp; BOM!B18</f>
-        <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="K17" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B18" s="15" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>59</v>
+      <c r="D18" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="17" t="n">
-        <v>729</v>
+        <v>979</v>
       </c>
       <c r="I18" s="17" t="n">
         <f aca="false">H18*C18</f>
-        <v>729</v>
+        <v>979</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="n">
+      <c r="K18" s="15" t="str">
+        <f aca="false">"Can be substituted with " &amp; BOM!B20</f>
+        <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21"/>
+      <c r="B19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="15" t="n">
         <v>1</v>
       </c>
+      <c r="D19" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="17" t="n">
+        <v>322.58</v>
+      </c>
+      <c r="I19" s="17" t="n">
+        <f aca="false">C19*H19</f>
+        <v>322.58</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="15" t="n">
-        <v>63197</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>68</v>
-      </c>
+      <c r="D20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="15"/>
       <c r="H20" s="17" t="n">
-        <v>351.2</v>
+        <v>729</v>
       </c>
       <c r="I20" s="17" t="n">
-        <f aca="false">C20*H20</f>
-        <v>351.2</v>
+        <f aca="false">H20*C20</f>
+        <v>729</v>
       </c>
       <c r="J20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="15" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="27"/>
+      <c r="B22" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="15" t="n">
-        <v>433122</v>
-      </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="17" t="n">
-        <v>359.2</v>
-      </c>
-      <c r="I21" s="17" t="n">
-        <f aca="false">C21*H21</f>
-        <v>359.2</v>
-      </c>
-      <c r="J21" s="15" t="s">
+      <c r="D22" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="31" t="n">
+        <v>75.44</v>
+      </c>
+      <c r="I22" s="31" t="n">
+        <f aca="false">C22*H22</f>
+        <v>75.44</v>
+      </c>
+      <c r="J22" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="n">
+      <c r="K22" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="27"/>
+      <c r="B23" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="15" t="n">
+      <c r="D23" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="31" t="n">
+        <v>40.48</v>
+      </c>
+      <c r="I23" s="31" t="n">
+        <f aca="false">C23*H23</f>
+        <v>40.48</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" s="17" t="n">
-        <v>146.925</v>
-      </c>
-      <c r="I23" s="17" t="n">
-        <f aca="false">C23*H23</f>
-        <v>146.925</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24"/>
-      <c r="B24" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17" t="n">
-        <f aca="false">C24*H24</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24"/>
       <c r="B25" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="C25" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="15" t="n">
+        <v>63197</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="17" t="n">
+        <v>351.2</v>
+      </c>
       <c r="I25" s="17" t="n">
         <f aca="false">C25*H25</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="15"/>
+        <v>351.2</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="K25" s="15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24"/>
+      <c r="A26" s="14" t="n">
+        <v>2</v>
+      </c>
       <c r="B26" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+        <v>86</v>
+      </c>
+      <c r="C26" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="15" t="n">
+        <v>433122</v>
+      </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="17" t="n">
+        <v>359.2</v>
+      </c>
       <c r="I26" s="17" t="n">
         <f aca="false">C26*H26</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="15"/>
+        <v>359.2</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="K26" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24"/>
-      <c r="B27" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17" t="n">
-        <f aca="false">C27*H27</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24"/>
-      <c r="B28" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="17"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="17" t="n">
+        <v>146.925</v>
+      </c>
       <c r="I28" s="17" t="n">
         <f aca="false">C28*H28</f>
+        <v>146.925</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="32"/>
+      <c r="B29" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17" t="n">
+        <f aca="false">C29*H29</f>
         <v>0</v>
       </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="21"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17" t="n">
+        <f aca="false">C30*H30</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="32"/>
+      <c r="B31" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17" t="n">
+        <f aca="false">C31*H31</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="32"/>
       <c r="B32" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H32" s="17" t="n">
-        <v>224.4</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="17"/>
       <c r="I32" s="17" t="n">
         <f aca="false">C32*H32</f>
-        <v>897.6</v>
+        <v>0</v>
       </c>
       <c r="J32" s="15"/>
-      <c r="K32" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="K32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="H33" s="17" t="n">
-        <v>198.352</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="17"/>
       <c r="I33" s="17" t="n">
         <f aca="false">C33*H33</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="21"/>
+      <c r="B37" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="25"/>
+      <c r="F37" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="17" t="n">
+        <v>224.4</v>
+      </c>
+      <c r="I37" s="17" t="n">
+        <f aca="false">C37*H37</f>
+        <v>897.6</v>
+      </c>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38" s="17" t="n">
+        <v>198.352</v>
+      </c>
+      <c r="I38" s="17" t="n">
+        <f aca="false">C38*H38</f>
         <v>793.408</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="19"/>
-      <c r="B34" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="15" t="n">
-        <v>24</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H34" s="17" t="n">
-        <v>309</v>
-      </c>
-      <c r="I34" s="17" t="n">
-        <f aca="false">C34*H34</f>
-        <v>7416</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="K34" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21"/>
-      <c r="B36" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" s="15" t="n">
-        <v>2536030320001</v>
-      </c>
-      <c r="H36" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="17" t="n">
-        <f aca="false">C36*H36</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21"/>
-      <c r="B38" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="17" t="n">
-        <v>369</v>
-      </c>
-      <c r="I38" s="17" t="n">
-        <f aca="false">H38*C38</f>
-        <v>369</v>
       </c>
       <c r="J38" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="26" t="str">
-        <f aca="false">"Needs to be ordered with " &amp; BOM!B17 &amp; "or " &amp; BOM!B18</f>
-        <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
+      <c r="K38" s="15" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="19"/>
       <c r="B39" s="15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C39" s="15" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>109</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E39" s="15"/>
       <c r="F39" s="16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H39" s="17" t="n">
-        <v>605.13</v>
+        <v>309</v>
       </c>
       <c r="I39" s="17" t="n">
         <f aca="false">C39*H39</f>
-        <v>605.13</v>
+        <v>7416</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2311,590 +2405,715 @@
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="21"/>
       <c r="B41" s="15" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C41" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="15" t="n">
-        <v>41015028</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G41" s="15"/>
+        <v>10</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="15" t="n">
+        <v>2536030320001</v>
+      </c>
       <c r="H41" s="17" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="I41" s="17" t="n">
-        <f aca="false">H41*C41</f>
-        <v>99</v>
+        <f aca="false">C41*H41</f>
+        <v>0</v>
       </c>
       <c r="J41" s="15" t="s">
         <v>20</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15"/>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="21"/>
+      <c r="B43" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="15"/>
+      <c r="H43" s="17" t="n">
+        <v>369</v>
+      </c>
+      <c r="I43" s="17" t="n">
+        <f aca="false">H43*C43</f>
+        <v>369</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" s="34" t="str">
+        <f aca="false">"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B20</f>
+        <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="19"/>
+      <c r="B44" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" s="17" t="n">
+        <v>605.13</v>
+      </c>
+      <c r="I44" s="17" t="n">
+        <f aca="false">C44*H44</f>
+        <v>605.13</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="21"/>
+      <c r="B46" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="15" t="n">
+        <v>41015028</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="G46" s="15"/>
+      <c r="H46" s="17" t="n">
+        <v>99</v>
+      </c>
+      <c r="I46" s="17" t="n">
+        <f aca="false">H46*C46</f>
+        <v>99</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15"/>
+      <c r="B48" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J48" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K48" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24"/>
-      <c r="B45" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="24"/>
-      <c r="B46" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24"/>
-      <c r="B47" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="24"/>
-      <c r="B48" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="24"/>
-      <c r="B49" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15" t="s">
-        <v>79</v>
-      </c>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="21"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C50" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="E50" s="15" t="n">
-        <v>41019265</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
-      <c r="H50" s="17" t="n">
-        <v>18</v>
-      </c>
-      <c r="I50" s="17" t="n">
-        <f aca="false">C50*H50</f>
-        <v>72</v>
-      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-    </row>
-    <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="24"/>
+      <c r="K50" s="15"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="32"/>
+      <c r="B51" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="32"/>
       <c r="B52" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E52" s="28" t="n">
-        <v>173010335</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>103</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="H52" s="17"/>
       <c r="I52" s="17"/>
-      <c r="J52" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="J52" s="15"/>
       <c r="K52" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="32"/>
       <c r="B53" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E53" s="28" t="n">
-        <v>173010542</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>103</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="H53" s="17"/>
       <c r="I53" s="17"/>
-      <c r="J53" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="J53" s="15"/>
       <c r="K53" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="32"/>
       <c r="B54" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C54" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D54" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E54" s="15" t="n">
-        <v>173011235</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>103</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
       <c r="G54" s="15"/>
-      <c r="H54" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="H54" s="17"/>
       <c r="I54" s="17"/>
-      <c r="J54" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="J54" s="15"/>
       <c r="K54" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="24"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="21"/>
       <c r="B55" s="15" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C55" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E55" s="28" t="n">
-        <v>173011535</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>103</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" s="15" t="n">
+        <v>41019265</v>
+      </c>
+      <c r="F55" s="15"/>
       <c r="G55" s="15"/>
       <c r="H55" s="17" t="n">
+        <v>18</v>
+      </c>
+      <c r="I55" s="17" t="n">
+        <f aca="false">C55*H55</f>
+        <v>72</v>
+      </c>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+    </row>
+    <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="32"/>
+      <c r="B57" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="35" t="n">
+        <v>173010335</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" s="15"/>
+      <c r="H57" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="I55" s="17"/>
-      <c r="J55" s="15" t="s">
+      <c r="I57" s="17"/>
+      <c r="J57" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K55" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="15"/>
-      <c r="B57" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" s="4" t="s">
+      <c r="K57" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="32"/>
+      <c r="B58" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K57" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="21"/>
+      <c r="D58" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="35" t="n">
+        <v>173010542</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" s="15"/>
+      <c r="H58" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="17"/>
+      <c r="J58" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="32"/>
       <c r="B59" s="15" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C59" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>136</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E59" s="15" t="n">
+        <v>173011235</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" s="15"/>
       <c r="H59" s="17" t="n">
-        <v>262.83</v>
-      </c>
-      <c r="I59" s="17" t="n">
-        <f aca="false">C59*H59</f>
-        <v>1576.98</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I59" s="17"/>
       <c r="J59" s="15" t="s">
         <v>20</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14"/>
-      <c r="B60" s="18" t="s">
-        <v>138</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="32"/>
+      <c r="B60" s="15" t="s">
+        <v>148</v>
       </c>
       <c r="C60" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="E60" s="15" t="n">
-        <v>5901259432770</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>141</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60" s="35" t="n">
+        <v>173011535</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" s="15"/>
       <c r="H60" s="17" t="n">
-        <v>237</v>
-      </c>
-      <c r="I60" s="17" t="n">
-        <f aca="false">C60*H60</f>
-        <v>237</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I60" s="17"/>
       <c r="J60" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K60" s="15"/>
-    </row>
-    <row r="64" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C64" s="30" t="n">
-        <f aca="false">SUM(I4,I9,I11,I12,I17,I20,I23,I32,I38,I41,I50)</f>
+      <c r="K60" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15"/>
+      <c r="B62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="21"/>
+      <c r="B64" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" s="15"/>
+      <c r="F64" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H64" s="17" t="n">
+        <v>262.83</v>
+      </c>
+      <c r="I64" s="17" t="n">
+        <f aca="false">C64*H64</f>
+        <v>1576.98</v>
+      </c>
+      <c r="J64" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K64" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="14"/>
+      <c r="B65" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E65" s="15" t="n">
+        <v>5901259432770</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="H65" s="17" t="n">
+        <v>237</v>
+      </c>
+      <c r="I65" s="17" t="n">
+        <f aca="false">C65*H65</f>
+        <v>237</v>
+      </c>
+      <c r="J65" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K65" s="15"/>
+    </row>
+    <row r="69" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="37" t="n">
+        <f aca="false">SUM(I4,I9,I11,I12,I18,I25,I28,I37,I43,I46,I55)</f>
         <v>6886.275</v>
       </c>
-      <c r="E64" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="F64" s="31"/>
-      <c r="G64" s="32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F65" s="21"/>
-      <c r="G65" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F66" s="14"/>
-      <c r="G66" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="F67" s="19"/>
-      <c r="G67" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="F68" s="24"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="15" t="s">
-        <v>154</v>
+      <c r="E69" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F70" s="21"/>
+      <c r="G70" s="15" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="15" t="s">
-        <v>155</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="15" t="s">
-        <v>156</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F72" s="19"/>
+      <c r="G72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="15" t="s">
-        <v>157</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="15" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="15" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A29:K29"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="A49:K49"/>
     <mergeCell ref="A56:K56"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A61:K61"/>
+    <mergeCell ref="A63:K63"/>
+    <mergeCell ref="E69:F69"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId2" display="Nanotec"/>
@@ -2908,37 +3127,46 @@
     <hyperlink ref="F11" r:id="rId10" display="STMICROELECTRONICS"/>
     <hyperlink ref="D12" r:id="rId11" display="Mouser"/>
     <hyperlink ref="F12" r:id="rId12" display="Vishay"/>
-    <hyperlink ref="D13" r:id="rId13" display="HobbyKing"/>
-    <hyperlink ref="D14" r:id="rId14" display="HobbyKing"/>
-    <hyperlink ref="D16" r:id="rId15" display="Amazon"/>
-    <hyperlink ref="D17" r:id="rId16" display="Electro:kit"/>
-    <hyperlink ref="D18" r:id="rId17" display="Electro:kit"/>
-    <hyperlink ref="D20" r:id="rId18" display="Elefun"/>
-    <hyperlink ref="F20" r:id="rId19" display="GNB"/>
-    <hyperlink ref="D21" r:id="rId20" display="Droneit"/>
-    <hyperlink ref="D23" r:id="rId21" display="Digikey"/>
-    <hyperlink ref="F23" r:id="rId22" display="Analog-devices"/>
-    <hyperlink ref="D32" r:id="rId23" display="Symmetry Electronics"/>
-    <hyperlink ref="F32" r:id="rId24" location="documents" display="iC-Haus"/>
-    <hyperlink ref="D33" r:id="rId25" display="Mouser"/>
-    <hyperlink ref="F33" r:id="rId26" display="Same sky"/>
-    <hyperlink ref="D34" r:id="rId27" display="Farnell"/>
-    <hyperlink ref="F34" r:id="rId28" display="BROADCOM"/>
-    <hyperlink ref="D36" r:id="rId29" display="Würth Electronic"/>
-    <hyperlink ref="F36" r:id="rId30" display="Würth Elektronik"/>
-    <hyperlink ref="D38" r:id="rId31" display="Electro:kit"/>
-    <hyperlink ref="D39" r:id="rId32" display="Mouser"/>
-    <hyperlink ref="F39" r:id="rId33" display="Texas Instruments"/>
-    <hyperlink ref="D41" r:id="rId34" display="Electro:kit"/>
-    <hyperlink ref="D50" r:id="rId35" display="Electrokit"/>
-    <hyperlink ref="D52" r:id="rId36" display="Würth Electronic"/>
-    <hyperlink ref="D53" r:id="rId37" display="Würth Electronic"/>
-    <hyperlink ref="D54" r:id="rId38" display="Würth Electronic"/>
-    <hyperlink ref="D55" r:id="rId39" display="Würth Electronic"/>
-    <hyperlink ref="D59" r:id="rId40" display="Farnell"/>
-    <hyperlink ref="F59" r:id="rId41" display="LEDEX"/>
-    <hyperlink ref="D60" r:id="rId42" display="Autodoc"/>
-    <hyperlink ref="F60" r:id="rId43" display="AS-PL"/>
+    <hyperlink ref="D13" r:id="rId13" display="Mouser"/>
+    <hyperlink ref="F13" r:id="rId14" display="STMicroelectronics"/>
+    <hyperlink ref="K13" r:id="rId15" display="Datasheet"/>
+    <hyperlink ref="D14" r:id="rId16" display="HobbyKing"/>
+    <hyperlink ref="D15" r:id="rId17" display="HobbyKing"/>
+    <hyperlink ref="D17" r:id="rId18" display="Amazon"/>
+    <hyperlink ref="D18" r:id="rId19" display="Electro:kit"/>
+    <hyperlink ref="D19" r:id="rId20" display="Mouser"/>
+    <hyperlink ref="F19" r:id="rId21" display="STMicroelectronics"/>
+    <hyperlink ref="D20" r:id="rId22" display="Electro:kit"/>
+    <hyperlink ref="D22" r:id="rId23" display="Mouser"/>
+    <hyperlink ref="F22" r:id="rId24" display="Semtech"/>
+    <hyperlink ref="D23" r:id="rId25" display="Mouser"/>
+    <hyperlink ref="F23" r:id="rId26" display="Skyworks Solutions, Inc."/>
+    <hyperlink ref="D25" r:id="rId27" display="Elefun"/>
+    <hyperlink ref="F25" r:id="rId28" display="GNB"/>
+    <hyperlink ref="D26" r:id="rId29" display="Droneit"/>
+    <hyperlink ref="D28" r:id="rId30" display="Digikey"/>
+    <hyperlink ref="F28" r:id="rId31" display="Analog-devices"/>
+    <hyperlink ref="D37" r:id="rId32" display="Symmetry Electronics"/>
+    <hyperlink ref="F37" r:id="rId33" location="documents" display="iC-Haus"/>
+    <hyperlink ref="D38" r:id="rId34" display="Mouser"/>
+    <hyperlink ref="F38" r:id="rId35" display="Same sky"/>
+    <hyperlink ref="D39" r:id="rId36" display="Farnell"/>
+    <hyperlink ref="F39" r:id="rId37" display="BROADCOM"/>
+    <hyperlink ref="D41" r:id="rId38" display="Würth Electronic"/>
+    <hyperlink ref="F41" r:id="rId39" display="Würth Elektronik"/>
+    <hyperlink ref="D43" r:id="rId40" display="Electro:kit"/>
+    <hyperlink ref="D44" r:id="rId41" display="Mouser"/>
+    <hyperlink ref="F44" r:id="rId42" display="Texas Instruments"/>
+    <hyperlink ref="D46" r:id="rId43" display="Electro:kit"/>
+    <hyperlink ref="D55" r:id="rId44" display="Electrokit"/>
+    <hyperlink ref="D57" r:id="rId45" display="Würth Electronic"/>
+    <hyperlink ref="D58" r:id="rId46" display="Würth Electronic"/>
+    <hyperlink ref="D59" r:id="rId47" display="Würth Electronic"/>
+    <hyperlink ref="D60" r:id="rId48" display="Würth Electronic"/>
+    <hyperlink ref="D64" r:id="rId49" display="Farnell"/>
+    <hyperlink ref="F64" r:id="rId50" display="LEDEX"/>
+    <hyperlink ref="D65" r:id="rId51" display="Autodoc"/>
+    <hyperlink ref="F65" r:id="rId52" display="AS-PL"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2947,6 +3175,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId44"/>
+  <legacyDrawing r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ranking color of B-G431B-ESC1
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -762,7 +762,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -815,13 +815,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -973,11 +966,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,63 +1063,35 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1326,10 +1291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1339,7 +1304,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="7.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="14.24"/>
@@ -1675,7 +1640,7 @@
       </c>
     </row>
     <row r="13" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="8" t="s">
         <v>48</v>
       </c>
@@ -1702,7 +1667,7 @@
         <v>1044.8</v>
       </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1892,7 +1857,7 @@
       <c r="C20" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="23" t="s">
         <v>63</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -1916,7 +1881,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>72</v>
       </c>
@@ -1931,71 +1896,71 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28" t="s">
+    <row r="22" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="24"/>
+      <c r="B22" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="28" t="n">
+      <c r="C22" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="31" t="n">
+      <c r="H22" s="17" t="n">
         <v>75.44</v>
       </c>
-      <c r="I22" s="31" t="n">
+      <c r="I22" s="17" t="n">
         <f aca="false">C22*H22</f>
         <v>75.44</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28" t="s">
+    <row r="23" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="24"/>
+      <c r="B23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="28" t="n">
+      <c r="C23" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G23" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="31" t="n">
+      <c r="H23" s="17" t="n">
         <v>40.48</v>
       </c>
-      <c r="I23" s="31" t="n">
+      <c r="I23" s="17" t="n">
         <f aca="false">C23*H23</f>
         <v>40.48</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="J23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="28" t="s">
+      <c r="K23" s="15" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2134,7 +2099,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="32"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="15" t="s">
         <v>95</v>
       </c>
@@ -2154,7 +2119,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="32"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="15" t="s">
         <v>97</v>
       </c>
@@ -2174,7 +2139,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="32"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="15" t="s">
         <v>98</v>
       </c>
@@ -2194,7 +2159,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="32"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="15" t="s">
         <v>99</v>
       </c>
@@ -2212,7 +2177,7 @@
       <c r="K32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="15" t="s">
         <v>100</v>
       </c>
@@ -2302,11 +2267,11 @@
       <c r="C37" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="33" t="s">
+      <c r="E37" s="23"/>
+      <c r="F37" s="26" t="s">
         <v>105</v>
       </c>
       <c r="G37" s="15" t="s">
@@ -2480,7 +2445,7 @@
       <c r="J43" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K43" s="34" t="str">
+      <c r="K43" s="27" t="str">
         <f aca="false">"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B20</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
@@ -2542,7 +2507,7 @@
       <c r="C46" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D46" s="25" t="s">
+      <c r="D46" s="23" t="s">
         <v>63</v>
       </c>
       <c r="E46" s="15" t="n">
@@ -2628,7 +2593,7 @@
       <c r="K49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="32"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="15" t="s">
         <v>135</v>
       </c>
@@ -2643,7 +2608,7 @@
       <c r="K50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="32"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="15" t="s">
         <v>136</v>
       </c>
@@ -2660,7 +2625,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="32"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="15" t="s">
         <v>138</v>
       </c>
@@ -2677,7 +2642,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="32"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="15" t="s">
         <v>139</v>
       </c>
@@ -2694,7 +2659,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="32"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="15" t="s">
         <v>140</v>
       </c>
@@ -2754,17 +2719,17 @@
       <c r="K56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="32"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="15" t="s">
         <v>144</v>
       </c>
       <c r="C57" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="E57" s="35" t="n">
+      <c r="E57" s="28" t="n">
         <v>173010335</v>
       </c>
       <c r="F57" s="15" t="s">
@@ -2783,17 +2748,17 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="32"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D58" s="25" t="s">
+      <c r="D58" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="E58" s="35" t="n">
+      <c r="E58" s="28" t="n">
         <v>173010542</v>
       </c>
       <c r="F58" s="15" t="s">
@@ -2812,14 +2777,14 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="32"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="15" t="s">
         <v>147</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="23" t="s">
         <v>119</v>
       </c>
       <c r="E59" s="15" t="n">
@@ -2841,17 +2806,17 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="32"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="15" t="s">
         <v>148</v>
       </c>
       <c r="C60" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D60" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="35" t="n">
+      <c r="E60" s="28" t="n">
         <v>173011535</v>
       </c>
       <c r="F60" s="15" t="s">
@@ -2997,23 +2962,23 @@
       <c r="K65" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="37" t="n">
+      <c r="C69" s="30" t="n">
         <f aca="false">SUM(I4,I9,I11,I12,I18,I25,I28,I37,I43,I46,I55)</f>
         <v>6886.275</v>
       </c>
-      <c r="E69" s="38" t="s">
+      <c r="E69" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39" t="s">
+      <c r="F69" s="31"/>
+      <c r="G69" s="32" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="33" t="s">
         <v>162</v>
       </c>
       <c r="E70" s="15" t="s">
@@ -3051,7 +3016,7 @@
       <c r="E73" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="F73" s="32"/>
+      <c r="F73" s="25"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="15" t="s">
@@ -3093,6 +3058,7 @@
         <v>117</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
Changed ranking of the wheel encoders and calculated sum for 1 robot
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="170">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">DF45L024048-A</t>
   </si>
   <si>
-    <t xml:space="preserve">In stock: 1 week</t>
+    <t xml:space="preserve">In stock</t>
   </si>
   <si>
     <t xml:space="preserve">BLDC motors for the wheels, compact size, light weight, contains hall sensors for encoder feedback
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">HobbyKing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">In stock</t>
   </si>
   <si>
     <t xml:space="preserve">Wheel BLDC
@@ -492,7 +489,7 @@
     <t xml:space="preserve">AEDB-9140-A13</t>
   </si>
   <si>
-    <t xml:space="preserve">Stock arriving week commencing 30/10/24</t>
+    <t xml:space="preserve">Stock arriving week commencing 13/10/24</t>
   </si>
   <si>
     <t xml:space="preserve">Wheel encoder, Quotation for 309 á excluding tax</t>
@@ -510,7 +507,7 @@
     <t xml:space="preserve">Würth Elektronik</t>
   </si>
   <si>
-    <t xml:space="preserve">IMU, Sponsored by W/E</t>
+    <t xml:space="preserve">IMU, Sponsored by W/E, Gyroscope, Acceleration, I2C, SPI</t>
   </si>
   <si>
     <t xml:space="preserve">Obsticle Detection Sensors</t>
@@ -738,19 +735,7 @@
     <t xml:space="preserve">3D printing costs</t>
   </si>
   <si>
-    <t xml:space="preserve">IR Sensors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hall Effect Sensors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ultrasonic sensors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lidar sensors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature sensors</t>
+    <t xml:space="preserve">Resistor and other passive components, sponsored by Würth</t>
   </si>
 </sst>
 </file>
@@ -970,7 +955,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1057,10 +1042,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1291,21 +1272,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="71.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="7.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="14.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.63"/>
@@ -1435,10 +1416,10 @@
         <v>1188</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,19 +1427,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="17" t="n">
@@ -1469,10 +1450,10 @@
         <v>861.6</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,13 +1461,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="15" t="n">
         <v>54896</v>
@@ -1501,15 +1482,15 @@
         <v>1075.2</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1523,24 +1504,26 @@
       <c r="K8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21"/>
+      <c r="A9" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B9" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="15" t="n">
         <v>65193</v>
       </c>
       <c r="F9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="H9" s="17" t="n">
         <v>175.2</v>
@@ -1550,15 +1533,15 @@
         <v>175.2</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1572,24 +1555,26 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
+      <c r="A11" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="B11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="G11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="9" t="n">
         <v>56.61</v>
@@ -1599,31 +1584,33 @@
         <v>283.05</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K11" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="12" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-      <c r="B12" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>30</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="H12" s="9" t="n">
         <v>7.99</v>
@@ -1633,31 +1620,33 @@
         <v>239.7</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K12" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="13" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
-      <c r="B13" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="C13" s="9" t="n">
         <v>5</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="G13" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="9" t="n">
         <v>208.96</v>
@@ -1668,7 +1657,7 @@
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,16 +1665,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="15" t="n">
         <v>5</v>
       </c>
       <c r="D14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -1697,10 +1686,10 @@
         <v>736</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,16 +1697,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
@@ -1729,15 +1718,15 @@
         <v>619.232</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1751,17 +1740,17 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="n">
-        <v>1</v>
+      <c r="A17" s="14" t="n">
+        <v>2</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1774,10 +1763,10 @@
         <v>203.2</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,19 +1774,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="F18" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>65</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="17" t="n">
@@ -1808,7 +1797,7 @@
         <v>979</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K18" s="15" t="str">
         <f aca="false">"Can be substituted with " &amp; BOM!B20</f>
@@ -1816,24 +1805,26 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21"/>
+      <c r="A19" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B19" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H19" s="17" t="n">
         <v>322.58</v>
@@ -1843,28 +1834,28 @@
         <v>322.58</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>63</v>
+      <c r="D20" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="17" t="n">
@@ -1875,15 +1866,15 @@
         <v>729</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1897,24 +1888,24 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>43</v>
+      <c r="D22" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="E22" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="16" t="s">
-        <v>75</v>
-      </c>
       <c r="G22" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H22" s="17" t="n">
         <v>75.44</v>
@@ -1924,31 +1915,31 @@
         <v>75.44</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K22" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23"/>
+      <c r="B23" s="15" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="23" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24"/>
-      <c r="B23" s="15" t="s">
-        <v>77</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>43</v>
+      <c r="D23" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="E23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="G23" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>80</v>
       </c>
       <c r="H23" s="17" t="n">
         <v>40.48</v>
@@ -1958,15 +1949,15 @@
         <v>40.48</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1984,22 +1975,22 @@
         <v>1</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="15" t="n">
         <v>63197</v>
       </c>
       <c r="F25" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="H25" s="17" t="n">
         <v>351.2</v>
@@ -2009,10 +2000,10 @@
         <v>351.2</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2020,13 +2011,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" s="15" t="n">
         <v>433122</v>
@@ -2041,15 +2032,15 @@
         <v>359.2</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -2067,22 +2058,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="F28" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="G28" s="15" t="s">
         <v>92</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>93</v>
       </c>
       <c r="H28" s="17" t="n">
         <v>146.925</v>
@@ -2092,16 +2083,16 @@
         <v>146.925</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K28" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="24"/>
+      <c r="B29" s="15" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25"/>
-      <c r="B29" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -2115,13 +2106,13 @@
       </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="24"/>
+      <c r="B30" s="15" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25"/>
-      <c r="B30" s="15" t="s">
-        <v>97</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -2135,13 +2126,13 @@
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -2155,13 +2146,13 @@
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -2177,9 +2168,9 @@
       <c r="K32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -2196,7 +2187,7 @@
     </row>
     <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2246,7 +2237,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -2260,22 +2251,24 @@
       <c r="K36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21"/>
+      <c r="A37" s="19" t="n">
+        <v>3</v>
+      </c>
       <c r="B37" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="22"/>
+      <c r="F37" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="26" t="s">
+      <c r="G37" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>106</v>
       </c>
       <c r="H37" s="17" t="n">
         <v>224.4</v>
@@ -2286,28 +2279,30 @@
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="C38" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="G38" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="H38" s="17" t="n">
         <v>198.352</v>
@@ -2317,29 +2312,31 @@
         <v>793.408</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
+      <c r="A39" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B39" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C39" s="15" t="n">
         <v>24</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>114</v>
       </c>
       <c r="H39" s="17" t="n">
         <v>309</v>
@@ -2349,15 +2346,15 @@
         <v>7416</v>
       </c>
       <c r="J39" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="K39" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="K39" s="15" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2371,19 +2368,21 @@
       <c r="K40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="21"/>
+      <c r="A41" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B41" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G41" s="15" t="n">
         <v>2536030320001</v>
@@ -2396,15 +2395,15 @@
         <v>0</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2418,21 +2417,23 @@
       <c r="K42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="21"/>
+      <c r="A43" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B43" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C43" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="17" t="n">
@@ -2443,32 +2444,34 @@
         <v>369</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K43" s="27" t="str">
+        <v>16</v>
+      </c>
+      <c r="K43" s="26" t="str">
         <f aca="false">"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B20</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="19"/>
+      <c r="A44" s="19" t="n">
+        <v>3</v>
+      </c>
       <c r="B44" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C44" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E44" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="G44" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="H44" s="17" t="n">
         <v>605.13</v>
@@ -2478,15 +2481,15 @@
         <v>605.13</v>
       </c>
       <c r="J44" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2500,21 +2503,23 @@
       <c r="K45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21"/>
+      <c r="A46" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B46" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C46" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>63</v>
+      <c r="D46" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="E46" s="15" t="n">
         <v>41015028</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="17" t="n">
@@ -2525,15 +2530,15 @@
         <v>99</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2593,9 +2598,9 @@
       <c r="K49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="25"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -2608,9 +2613,9 @@
       <c r="K50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="25"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
@@ -2621,13 +2626,13 @@
       <c r="I51" s="17"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="24"/>
+      <c r="B52" s="15" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="25"/>
-      <c r="B52" s="15" t="s">
-        <v>138</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
@@ -2638,13 +2643,13 @@
       <c r="I52" s="17"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -2655,13 +2660,13 @@
       <c r="I53" s="17"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="25"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -2672,19 +2677,21 @@
       <c r="I54" s="17"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="21"/>
+      <c r="A55" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B55" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C55" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E55" s="15" t="n">
         <v>41019265</v>
@@ -2700,12 +2707,12 @@
       </c>
       <c r="J55" s="15"/>
       <c r="K55" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -2719,21 +2726,21 @@
       <c r="K56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="25"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C57" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="D57" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="27" t="n">
+        <v>173010335</v>
+      </c>
+      <c r="F57" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="E57" s="28" t="n">
-        <v>173010335</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>120</v>
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="17" t="n">
@@ -2741,28 +2748,28 @@
       </c>
       <c r="I57" s="17"/>
       <c r="J57" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K57" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="24"/>
+      <c r="B58" s="15" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
-      <c r="B58" s="15" t="s">
-        <v>146</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D58" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E58" s="27" t="n">
+        <v>173010542</v>
+      </c>
+      <c r="F58" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="E58" s="28" t="n">
-        <v>173010542</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>120</v>
       </c>
       <c r="G58" s="15"/>
       <c r="H58" s="17" t="n">
@@ -2770,28 +2777,28 @@
       </c>
       <c r="I58" s="17"/>
       <c r="J58" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D59" s="23" t="s">
-        <v>119</v>
+      <c r="D59" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="E59" s="15" t="n">
         <v>173011235</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="17" t="n">
@@ -2799,28 +2806,28 @@
       </c>
       <c r="I59" s="17"/>
       <c r="J59" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="25"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D60" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E60" s="27" t="n">
+        <v>173011535</v>
+      </c>
+      <c r="F60" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="E60" s="28" t="n">
-        <v>173011535</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>120</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="17" t="n">
@@ -2828,15 +2835,15 @@
       </c>
       <c r="I60" s="17"/>
       <c r="J60" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2884,7 +2891,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -2898,22 +2905,24 @@
       <c r="K63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="21"/>
+      <c r="A64" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B64" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C64" s="15" t="n">
         <v>6</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G64" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="G64" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="H64" s="17" t="n">
         <v>262.83</v>
@@ -2923,31 +2932,31 @@
         <v>1576.98</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="14"/>
       <c r="B65" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C65" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E65" s="15" t="n">
         <v>5901259432770</v>
       </c>
       <c r="F65" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G65" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="G65" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="H65" s="17" t="n">
         <v>237</v>
@@ -2957,108 +2966,99 @@
         <v>237</v>
       </c>
       <c r="J65" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K65" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="29" t="n">
+        <f aca="false">SUM(I4,I9,I13,I18,I19,I22,I23,I25,I28,I39,I43,I46,I55)</f>
+        <v>14365.225</v>
+      </c>
+      <c r="E69" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="30" t="n">
-        <f aca="false">SUM(I4,I9,I11,I12,I18,I25,I28,I37,I43,I46,I55)</f>
-        <v>6886.275</v>
-      </c>
-      <c r="E69" s="31" t="s">
+      <c r="F69" s="30"/>
+      <c r="G69" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="F69" s="31"/>
-      <c r="G69" s="32" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="32" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="33" t="s">
+      <c r="E70" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E71" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="E71" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="F73" s="25"/>
+        <v>167</v>
+      </c>
+      <c r="F73" s="24"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="15" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="15" t="s">
-        <v>172</v>
-      </c>
+      <c r="B78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="15" t="s">
-        <v>173</v>
-      </c>
+      <c r="B79" s="26"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="15" t="s">
-        <v>174</v>
-      </c>
+      <c r="B80" s="26"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B81" s="26"/>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
Added components to the BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6105D996-0280-4D62-8580-0D03DDE561E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5897BD1C-B29E-42EC-98CE-E2E6A524BE5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="H58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="196">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -742,14 +742,89 @@
     <t>Resistor and other passive components, sponsored by Würth</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Signal-transformers</t>
+  </si>
+  <si>
+    <t>Ljudtransformatorer/Signaltransformatorer DA2032 Cap Chrgr For Linear LT3750/51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DA2034-ALD (Recomennded transformer) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MURS140-13-F (Recommended diod) </t>
+  </si>
+  <si>
+    <t>DIODE GEN PURP 400V 1A SMB</t>
+  </si>
+  <si>
+    <t>Passive-components</t>
+  </si>
+  <si>
+    <t>Discrete-semiconductor-products</t>
+  </si>
+  <si>
+    <t>ALC80A181CB400</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>GRM3195C2A363JA01D</t>
+  </si>
+  <si>
+    <t>GRM21BC8YA106KE11L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF7493TRPBF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSMN038-100YLX </t>
+  </si>
+  <si>
+    <t>PHT6NQ10T,135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420VXG180MEFCSN25X35  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.036UF 100V C0GNP0 1206. Bypass capacitor 56uF (0.036u+0.036u in series) </t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 35V X6S 0805. Bypass capacitor 10uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET N-CH 80V 9.3A 8SO. Recommended MOSFET </t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 100V 3A SOT223. Recommended MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET N-CH 100V 30A LFPAK56. Recommended MOSFET </t>
+  </si>
+  <si>
+    <t>CAP ALUM 180UF 20% 400V SNAP TH. Backup capacitor, capacitor 180uF</t>
+  </si>
+  <si>
+    <t>Aluminumelektrolytkondensatorer - snäppfäste LONG LIFE ALUMINUM ELECTROLYTIC CAPACITORS. Capacitor 180uF</t>
+  </si>
+  <si>
+    <t>C0603C330J2GAC7867</t>
+  </si>
+  <si>
+    <t>CAP CER 33PF 200V C0G/NP0 0603. Bypass capacitor 33pF</t>
+  </si>
+  <si>
+    <t>CR0603AFX-1003EAS</t>
+  </si>
+  <si>
+    <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Anti-Sulfur, Automotive AEC-Q200, Moisture Resistant Thick Film</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -852,6 +927,24 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -925,17 +1018,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -983,6 +1067,20 @@
     <xf numFmtId="4" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1179,1816 +1277,2162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="72" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="81.88671875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="72" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="81.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+    </row>
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <v>4</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="12">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="9">
         <v>818.4</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="9">
         <f>C4*H4</f>
         <v>3273.6</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="13" t="s">
+      <c r="J4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>4</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>9392000008</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="18">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="15">
         <v>297</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="15">
         <f>C5*H5</f>
         <v>1188</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="19" t="s">
+      <c r="J5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="17">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>4</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="18">
+      <c r="G6" s="13"/>
+      <c r="H6" s="15">
         <v>215.4</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="15">
         <f>C6*H6</f>
         <v>861.6</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="16" t="s">
+      <c r="J6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="17">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>4</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>54896</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="21">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="18">
         <v>268.8</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="15">
         <f>C7*H7</f>
         <v>1075.2</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>1</v>
-      </c>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="19">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>65193</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>175.2</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="15">
         <f>C9*H9</f>
         <v>175.2</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="16" t="s">
+      <c r="J9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>5</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>56.61</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <f>C11*H11</f>
         <v>283.05</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="9" t="s">
+      <c r="J11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>30</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>7.99</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <f>C12*H12</f>
         <v>239.70000000000002</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="9" t="s">
+      <c r="J12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>1</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>5</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <v>208.96</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="7">
         <f>C13*H13</f>
         <v>1044.8</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="11" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="A14" s="12">
         <v>2</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <v>5</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18">
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="15">
         <v>147.19999999999999</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="15">
         <f>C14*H14</f>
         <v>736</v>
       </c>
-      <c r="J14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="19" t="s">
+      <c r="J14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="A15" s="17">
         <v>3</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>4</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="18">
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="15">
         <v>154.80799999999999</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="15">
         <f>H15*C15</f>
         <v>619.23199999999997</v>
       </c>
-      <c r="J15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="16" t="s">
+      <c r="J15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="12">
         <v>2</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="16">
-        <v>1</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="18">
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="15">
         <v>203.2</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="15">
         <f>C17*H17</f>
         <v>203.2</v>
       </c>
-      <c r="J17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="16" t="s">
+      <c r="J17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>1</v>
-      </c>
-      <c r="B18" s="16" t="s">
+      <c r="A18" s="19">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="16">
-        <v>1</v>
-      </c>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="18">
+      <c r="G18" s="13"/>
+      <c r="H18" s="15">
         <v>979</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="15">
         <f>H18*C18</f>
         <v>979</v>
       </c>
-      <c r="J18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="16" t="str">
+      <c r="J18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="13" t="str">
         <f>"Can be substituted with " &amp; BOM!B20</f>
         <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>1</v>
-      </c>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="16">
-        <v>1</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="15">
         <v>322.58</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="15">
         <f>C19*H19</f>
         <v>322.58</v>
       </c>
-      <c r="J19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="19" t="s">
+      <c r="J19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="16">
-        <v>1</v>
-      </c>
-      <c r="D20" s="23" t="s">
+      <c r="C20" s="13">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="18">
+      <c r="G20" s="13"/>
+      <c r="H20" s="15">
         <v>729</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="15">
         <f>H20*C20</f>
         <v>729</v>
       </c>
-      <c r="J20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="16" t="s">
+      <c r="J20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="16" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
-      <c r="D22" s="23" t="s">
+      <c r="C22" s="13">
+        <v>1</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="15">
         <v>75.44</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="15">
         <f>C22*H22</f>
         <v>75.44</v>
       </c>
-      <c r="J22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="16" t="s">
+      <c r="J22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="16">
-        <v>1</v>
-      </c>
-      <c r="D23" s="23" t="s">
+      <c r="C23" s="13">
+        <v>1</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="15">
         <v>40.479999999999997</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="15">
         <f>C23*H23</f>
         <v>40.479999999999997</v>
       </c>
-      <c r="J23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="16" t="s">
+      <c r="J23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
-        <v>1</v>
-      </c>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="19">
+        <v>1</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="16">
-        <v>1</v>
-      </c>
-      <c r="D25" s="17" t="s">
+      <c r="C25" s="13">
+        <v>1</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="13">
         <v>63197</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="15">
         <v>351.2</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="15">
         <f>C25*H25</f>
         <v>351.2</v>
       </c>
-      <c r="J25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="16" t="s">
+      <c r="J25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="12">
         <v>2</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="16">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17" t="s">
+      <c r="C26" s="13">
+        <v>1</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="13">
         <v>433122</v>
       </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="18">
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="15">
         <v>359.2</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I26" s="15">
         <f>C26*H26</f>
         <v>359.2</v>
       </c>
-      <c r="J26" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="16" t="s">
+      <c r="J26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
     </row>
     <row r="28" spans="1:11" ht="184.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
-        <v>1</v>
-      </c>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="19">
+        <v>1</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="16">
-        <v>1</v>
-      </c>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="13">
+        <v>1</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="15">
         <v>146.92500000000001</v>
       </c>
-      <c r="I28" s="18">
-        <f t="shared" ref="I28:I33" si="0">C28*H28</f>
+      <c r="I28" s="15">
+        <f t="shared" ref="I28:I45" si="0">C28*H28</f>
         <v>146.92500000000001</v>
       </c>
-      <c r="J28" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="19" t="s">
+      <c r="J28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="19">
+        <v>1</v>
+      </c>
       <c r="B29" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="15">
+        <v>98.56</v>
+      </c>
+      <c r="I29" s="15">
+        <v>98.56</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="19">
+        <v>1</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="13">
+        <v>1</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="15">
+        <v>4.09</v>
+      </c>
+      <c r="I30" s="15">
+        <v>4.09</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="19">
+        <v>1</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="13">
+        <v>1</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="15">
+        <v>56.47</v>
+      </c>
+      <c r="I31" s="15">
+        <v>56.47</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="19">
+        <v>1</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="15">
+        <v>42.267800000000001</v>
+      </c>
+      <c r="I32" s="15">
+        <v>52.83475</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="19">
+        <v>1</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C33" s="13">
+        <v>1</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15">
+        <v>11.05</v>
+      </c>
+      <c r="I33" s="15">
+        <v>11.05</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="19">
+        <v>1</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="13">
+        <v>1</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="15">
+        <v>10.43</v>
+      </c>
+      <c r="I34" s="15">
+        <v>10.43</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="19">
+        <v>1</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" s="13">
+        <v>1</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="15">
+        <v>16.88</v>
+      </c>
+      <c r="I35" s="15">
+        <v>16.88</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="19">
+        <v>1</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="I36" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="19">
+        <v>1</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="13">
+        <v>2</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="15">
+        <v>5.63</v>
+      </c>
+      <c r="I37" s="15">
+        <v>5.63</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="19">
+        <v>1</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" s="13">
+        <v>1</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="I38" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" s="34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="19">
+        <v>1</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="I39" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="16"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18">
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16" t="s">
+      <c r="J41" s="13"/>
+      <c r="K41" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="16" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+      <c r="B42" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18">
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16" t="s">
+      <c r="J42" s="13"/>
+      <c r="K42" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="16" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18">
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16" t="s">
+      <c r="J43" s="13"/>
+      <c r="K43" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="16" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18">
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="16" t="s">
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+      <c r="B45" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18">
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-    </row>
-    <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+    </row>
+    <row r="46" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D47" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G47" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H47" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I47" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J47" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="K47" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="20">
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+    </row>
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="17">
         <v>3</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B49" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C49" s="13">
         <v>4</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D49" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="26" t="s">
+      <c r="E49" s="20"/>
+      <c r="F49" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G49" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H49" s="15">
         <v>224.4</v>
       </c>
-      <c r="I37" s="18">
-        <f>C37*H37</f>
+      <c r="I49" s="15">
+        <f>C49*H49</f>
         <v>897.6</v>
       </c>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16" t="s">
+      <c r="J49" s="13"/>
+      <c r="K49" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
         <v>2</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B50" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C50" s="13">
         <v>4</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D50" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E50" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F50" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="G50" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H50" s="15">
         <v>198.352</v>
       </c>
-      <c r="I38" s="18">
-        <f>C38*H38</f>
+      <c r="I50" s="15">
+        <f>C50*H50</f>
         <v>793.40800000000002</v>
       </c>
-      <c r="J38" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K38" s="16" t="s">
+      <c r="J50" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
-        <v>1</v>
-      </c>
-      <c r="B39" s="16" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="19">
+        <v>1</v>
+      </c>
+      <c r="B51" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C51" s="13">
         <v>24</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D51" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17" t="s">
+      <c r="E51" s="13"/>
+      <c r="F51" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="G51" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H51" s="15">
         <v>309</v>
       </c>
-      <c r="I39" s="18">
-        <f>C39*H39</f>
+      <c r="I51" s="15">
+        <f>C51*H51</f>
         <v>7416</v>
       </c>
-      <c r="J39" s="16" t="s">
+      <c r="J51" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K39" s="16" t="s">
+      <c r="K51" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
-        <v>1</v>
-      </c>
-      <c r="B41" s="16" t="s">
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="30"/>
+      <c r="K52" s="30"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="19">
+        <v>1</v>
+      </c>
+      <c r="B53" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C53" s="13">
         <v>10</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D53" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17" t="s">
+      <c r="E53" s="13"/>
+      <c r="F53" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G53" s="13">
         <v>2536030320001</v>
       </c>
-      <c r="H41" s="18">
+      <c r="H53" s="15">
         <v>0</v>
       </c>
-      <c r="I41" s="18">
-        <f>C41*H41</f>
+      <c r="I53" s="15">
+        <f>C53*H53</f>
         <v>0</v>
       </c>
-      <c r="J41" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K41" s="16" t="s">
+      <c r="J53" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K53" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A54" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
-        <v>1</v>
-      </c>
-      <c r="B43" s="16" t="s">
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="30"/>
+      <c r="K54" s="30"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="19">
+        <v>1</v>
+      </c>
+      <c r="B55" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="16">
-        <v>1</v>
-      </c>
-      <c r="D43" s="17" t="s">
+      <c r="C55" s="13">
+        <v>1</v>
+      </c>
+      <c r="D55" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E55" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F55" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="16"/>
-      <c r="H43" s="18">
+      <c r="G55" s="13"/>
+      <c r="H55" s="15">
         <v>369</v>
       </c>
-      <c r="I43" s="18">
-        <f>H43*C43</f>
+      <c r="I55" s="15">
+        <f>H55*C55</f>
         <v>369</v>
       </c>
-      <c r="J43" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="27" t="str">
+      <c r="J55" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" s="24" t="str">
         <f>"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B20</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
         <v>3</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B56" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C44" s="16">
-        <v>1</v>
-      </c>
-      <c r="D44" s="17" t="s">
+      <c r="C56" s="13">
+        <v>1</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E56" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F56" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="G56" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H56" s="15">
         <v>605.13</v>
       </c>
-      <c r="I44" s="18">
-        <f>C44*H44</f>
+      <c r="I56" s="15">
+        <f>C56*H56</f>
         <v>605.13</v>
       </c>
-      <c r="J44" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="16" t="s">
+      <c r="J56" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K56" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="22">
-        <v>1</v>
-      </c>
-      <c r="B46" s="16" t="s">
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="30"/>
+      <c r="J57" s="30"/>
+      <c r="K57" s="30"/>
+    </row>
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="19">
+        <v>1</v>
+      </c>
+      <c r="B58" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="16">
-        <v>1</v>
-      </c>
-      <c r="D46" s="23" t="s">
+      <c r="C58" s="13">
+        <v>1</v>
+      </c>
+      <c r="D58" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E58" s="13">
         <v>41015028</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F58" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="16"/>
-      <c r="H46" s="18">
+      <c r="G58" s="13"/>
+      <c r="H58" s="15">
         <v>99</v>
       </c>
-      <c r="I46" s="18">
-        <f>H46*C46</f>
+      <c r="I58" s="15">
+        <f>H58*C58</f>
         <v>99</v>
       </c>
-      <c r="J46" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="16" t="s">
+      <c r="J58" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="59" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="6" t="s">
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="31"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C60" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D60" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E60" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F60" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G60" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="H60" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I60" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="J60" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K48" s="6" t="s">
+      <c r="K60" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="16" t="s">
+    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="22"/>
+      <c r="B62" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="16" t="s">
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16" t="s">
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="16" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
+      <c r="B64" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16" t="s">
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
-      <c r="B53" s="16" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="22"/>
+      <c r="B65" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16" t="s">
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
-      <c r="B54" s="16" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="22"/>
+      <c r="B66" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16" t="s">
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
-        <v>1</v>
-      </c>
-      <c r="B55" s="16" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="19">
+        <v>1</v>
+      </c>
+      <c r="B67" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C67" s="13">
         <v>4</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D67" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="16">
+      <c r="E67" s="13">
         <v>41019265</v>
       </c>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="18">
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="15">
         <v>18</v>
       </c>
-      <c r="I55" s="18">
-        <f>C55*H55</f>
+      <c r="I67" s="15">
+        <f>C67*H67</f>
         <v>72</v>
       </c>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16" t="s">
+      <c r="J67" s="13"/>
+      <c r="K67" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="25"/>
-      <c r="B57" s="16" t="s">
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+    </row>
+    <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" s="22"/>
+      <c r="B69" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C69" s="13">
         <v>3</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="D69" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="28">
+      <c r="E69" s="25">
         <v>173010335</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="F69" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="18">
+      <c r="G69" s="13"/>
+      <c r="H69" s="15">
         <v>0</v>
       </c>
-      <c r="I57" s="18"/>
-      <c r="J57" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K57" s="16" t="s">
+      <c r="I69" s="15"/>
+      <c r="J69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="25"/>
-      <c r="B58" s="16" t="s">
+    <row r="70" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="22"/>
+      <c r="B70" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="16">
+      <c r="C70" s="13">
         <v>3</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D70" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E58" s="28">
+      <c r="E70" s="25">
         <v>173010542</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F70" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="18">
+      <c r="G70" s="13"/>
+      <c r="H70" s="15">
         <v>0</v>
       </c>
-      <c r="I58" s="18"/>
-      <c r="J58" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K58" s="16" t="s">
+      <c r="I70" s="15"/>
+      <c r="J70" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="25"/>
-      <c r="B59" s="16" t="s">
+    <row r="71" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="22"/>
+      <c r="B71" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C71" s="13">
         <v>3</v>
       </c>
-      <c r="D59" s="23" t="s">
+      <c r="D71" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="16">
+      <c r="E71" s="13">
         <v>173011235</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F71" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G59" s="16"/>
-      <c r="H59" s="18">
+      <c r="G71" s="13"/>
+      <c r="H71" s="15">
         <v>0</v>
       </c>
-      <c r="I59" s="18"/>
-      <c r="J59" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K59" s="16" t="s">
+      <c r="I71" s="15"/>
+      <c r="J71" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="25"/>
-      <c r="B60" s="16" t="s">
+    <row r="72" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="22"/>
+      <c r="B72" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="16">
+      <c r="C72" s="13">
         <v>3</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D72" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="28">
+      <c r="E72" s="25">
         <v>173011535</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F72" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G60" s="16"/>
-      <c r="H60" s="18">
+      <c r="G72" s="13"/>
+      <c r="H72" s="15">
         <v>0</v>
       </c>
-      <c r="I60" s="18"/>
-      <c r="J60" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="16" t="s">
+      <c r="I72" s="15"/>
+      <c r="J72" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+    <row r="73" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A73" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="6" t="s">
+      <c r="B73" s="31"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="31"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C74" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D74" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E74" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F74" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="G74" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="H74" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I74" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J62" s="6" t="s">
+      <c r="J74" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K62" s="6" t="s">
+      <c r="K74" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A75" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="22">
-        <v>1</v>
-      </c>
-      <c r="B64" s="16" t="s">
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="19">
+        <v>1</v>
+      </c>
+      <c r="B76" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="16">
+      <c r="C76" s="13">
         <v>6</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D76" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17" t="s">
+      <c r="E76" s="13"/>
+      <c r="F76" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G64" s="16" t="s">
+      <c r="G76" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="H64" s="18">
+      <c r="H76" s="15">
         <v>262.83</v>
       </c>
-      <c r="I64" s="18">
-        <f>C64*H64</f>
+      <c r="I76" s="15">
+        <f>C76*H76</f>
         <v>1576.98</v>
       </c>
-      <c r="J64" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K64" s="16" t="s">
+      <c r="J76" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K76" s="13" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="19" t="s">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="12"/>
+      <c r="B77" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C65" s="16">
-        <v>1</v>
-      </c>
-      <c r="D65" s="17" t="s">
+      <c r="C77" s="13">
+        <v>1</v>
+      </c>
+      <c r="D77" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="E65" s="16">
+      <c r="E77" s="13">
         <v>5901259432770</v>
       </c>
-      <c r="F65" s="17" t="s">
+      <c r="F77" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="G65" s="16" t="s">
+      <c r="G77" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="H65" s="18">
+      <c r="H77" s="15">
         <v>237</v>
       </c>
-      <c r="I65" s="18">
-        <f>C65*H65</f>
+      <c r="I77" s="15">
+        <f>C77*H77</f>
         <v>237</v>
       </c>
-      <c r="J65" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K65" s="16"/>
-    </row>
-    <row r="69" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B69" s="29" t="s">
+      <c r="J77" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="13"/>
+    </row>
+    <row r="81" spans="2:7" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B81" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="30">
-        <f>SUM(I4,I9,I13,I18,I19,I22,I23,I25,I28,I39,I43,I46,I55)</f>
+      <c r="C81" s="27">
+        <f>SUM(I4,I9,I13,I18,I19,I22,I23,I25,I28,I51,I55,I58,I67)</f>
         <v>14365.224999999999</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E81" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="31" t="s">
+      <c r="F81" s="32"/>
+      <c r="G81" s="28" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B70" s="32" t="s">
+    <row r="82" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B82" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E82" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="F70" s="22"/>
-      <c r="G70" s="16" t="s">
+      <c r="F82" s="19"/>
+      <c r="G82" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B71" s="16" t="s">
+    <row r="83" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B83" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E83" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F71" s="15"/>
-      <c r="G71" s="16"/>
-    </row>
-    <row r="72" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B72" s="16" t="s">
+      <c r="F83" s="12"/>
+      <c r="G83" s="13"/>
+    </row>
+    <row r="84" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B84" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E84" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="F72" s="20"/>
-      <c r="G72" s="16"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="16" t="s">
+      <c r="F84" s="17"/>
+      <c r="G84" s="13"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E85" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F73" s="25"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="16" t="s">
+      <c r="F85" s="22"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="16" t="s">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B76" s="16" t="s">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B77" s="16" t="s">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B78"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B79" s="27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B80" s="27"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="27"/>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="24"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="24"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A56:K56"/>
-    <mergeCell ref="A61:K61"/>
-    <mergeCell ref="A63:K63"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A73:K73"/>
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A61:K61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3021,34 +3465,54 @@
     <hyperlink ref="D26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="D28" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="F28" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F37" r:id="rId32" location="documents" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D38" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F38" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D41" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="F41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D43" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="D44" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D46" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D55" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D57" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D58" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D59" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D60" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="D64" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="F64" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D65" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="F65" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="D49" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F49" r:id="rId32" location="documents" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F50" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D51" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F51" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D53" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F53" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D55" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D56" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F56" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D58" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D67" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D69" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D70" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D71" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D72" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D76" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F76" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D77" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F77" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="D29" r:id="rId52" xr:uid="{876E345E-1D94-4A3A-B802-012FDED57481}"/>
+    <hyperlink ref="F29" r:id="rId53" xr:uid="{628119BE-F2D7-4277-A29F-A0FFDCCE110D}"/>
+    <hyperlink ref="D30" r:id="rId54" xr:uid="{BD7440CF-9727-473C-A25D-FB5A217BDA81}"/>
+    <hyperlink ref="F30" r:id="rId55" xr:uid="{17851481-F47B-4CB5-81CC-04E95AA70B73}"/>
+    <hyperlink ref="D31" r:id="rId56" xr:uid="{1828FD13-6BFF-4B01-914F-1BC233FECB5C}"/>
+    <hyperlink ref="F31" r:id="rId57" xr:uid="{8DEDCE52-2DC4-42CD-8402-B0EADE2EFCF0}"/>
+    <hyperlink ref="D32" r:id="rId58" xr:uid="{3C781D9D-8041-4FB9-A809-3FAEB2D4E236}"/>
+    <hyperlink ref="F32" r:id="rId59" xr:uid="{6E38FB9B-0E84-464D-B0E2-55CA261EF2E4}"/>
+    <hyperlink ref="D33" r:id="rId60" xr:uid="{93837A35-C019-4732-9FE6-0C3E51B6BAC6}"/>
+    <hyperlink ref="F33" r:id="rId61" xr:uid="{047D022A-DB19-4FE6-B236-86A5DEE46EF4}"/>
+    <hyperlink ref="D34" r:id="rId62" xr:uid="{1F1808A4-BD47-4E91-9C9E-54549BED3D2B}"/>
+    <hyperlink ref="F34" r:id="rId63" xr:uid="{7920FB48-F6C8-4A65-AC66-05454EF7B48C}"/>
+    <hyperlink ref="D35" r:id="rId64" xr:uid="{74FE0C9E-D7BE-404B-9644-33B4ADBB6E60}"/>
+    <hyperlink ref="F35" r:id="rId65" xr:uid="{9710C103-683A-41DC-ADA9-C05F9CF128C9}"/>
+    <hyperlink ref="D36" r:id="rId66" xr:uid="{0B1723FA-24AB-4E32-8F38-5CBCF269C63E}"/>
+    <hyperlink ref="F36" r:id="rId67" xr:uid="{9EF60CAE-95E9-49FB-8EB6-5C435632018B}"/>
+    <hyperlink ref="D37" r:id="rId68" xr:uid="{2B707495-F9E5-45BA-90A4-A9E8FF0708E3}"/>
+    <hyperlink ref="F37" r:id="rId69" xr:uid="{89F13473-EADE-4FC1-9A68-F9AC21EAA78B}"/>
+    <hyperlink ref="D38" r:id="rId70" xr:uid="{11380CE5-128C-470B-B728-27DF70A3633B}"/>
+    <hyperlink ref="D39" r:id="rId71" xr:uid="{4336C976-5B02-48FA-B06D-E8DE994D7146}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId72"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId52"/>
+  <legacyDrawing r:id="rId73"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added passive components in the BOM for the kicker
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5897BD1C-B29E-42EC-98CE-E2E6A524BE5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB14B822-2CB0-4B08-A95A-423DC6EC5505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,13 +69,13 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Incl. Moms</t>
         </r>
       </text>
     </comment>
-    <comment ref="H55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H62" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="H65" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="210">
   <si>
     <t>Powertrain and Electronics</t>
   </si>
@@ -819,12 +819,54 @@
   <si>
     <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Anti-Sulfur, Automotive AEC-Q200, Moisture Resistant Thick Film</t>
   </si>
+  <si>
+    <t>CRM2512QFX-1003ELF</t>
+  </si>
+  <si>
+    <t>100 kOhms ±1% 2W Chip Resistor 2512 (6432 Metric) Automotive AEC-Q200, Pulse Withstanding Thick Film</t>
+  </si>
+  <si>
+    <t>RC0603FR-0743RL</t>
+  </si>
+  <si>
+    <t>43 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-PA3J430V </t>
+  </si>
+  <si>
+    <t>43 Ohms ±5% 0.333W, 1/3W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200, Pulse Withstanding Thick Film</t>
+  </si>
+  <si>
+    <t>ERJ-3BWFR025V</t>
+  </si>
+  <si>
+    <t>25 mOhms ±1% 0.333W, 1/3W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200, Current Sense Thick Film</t>
+  </si>
+  <si>
+    <t>RCC120620K0FKEA</t>
+  </si>
+  <si>
+    <t>20 kOhms ±1% 0.5W, 1/2W Chip Resistor 1206 (3216 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>Würth Elektronik?</t>
+  </si>
+  <si>
+    <t>2.49 kOhms ±1% 0.1W, 1/10W Chip Resistor 0402 (1005 Metric) Anti-Sulfur Thick Film</t>
+  </si>
+  <si>
+    <t>MCWR06X2491FTL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -925,7 +967,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -935,12 +977,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1018,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
@@ -1067,20 +1103,19 @@
     <xf numFmtId="4" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1277,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="I33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1299,19 +1334,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1349,19 +1384,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -1494,19 +1529,19 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
@@ -1545,19 +1580,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1730,19 +1765,19 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -1878,19 +1913,19 @@
       </c>
     </row>
     <row r="21" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
     </row>
     <row r="22" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
@@ -1961,19 +1996,19 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
@@ -2044,19 +2079,19 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
     </row>
     <row r="28" spans="1:11" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
@@ -2084,7 +2119,7 @@
         <v>146.92500000000001</v>
       </c>
       <c r="I28" s="15">
-        <f t="shared" ref="I28:I45" si="0">C28*H28</f>
+        <f t="shared" ref="I28:I52" si="0">C28*H28</f>
         <v>146.92500000000001</v>
       </c>
       <c r="J28" s="13" t="s">
@@ -2104,11 +2139,11 @@
       <c r="C29" s="13">
         <v>1</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="13"/>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="30" t="s">
         <v>170</v>
       </c>
       <c r="G29" s="13"/>
@@ -2121,7 +2156,7 @@
       <c r="J29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="34" t="s">
+      <c r="K29" s="31" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2135,11 +2170,11 @@
       <c r="C30" s="13">
         <v>1</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E30" s="13"/>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="30" t="s">
         <v>176</v>
       </c>
       <c r="G30" s="13"/>
@@ -2152,7 +2187,7 @@
       <c r="J30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="36" t="s">
+      <c r="K30" s="33" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2166,11 +2201,11 @@
       <c r="C31" s="13">
         <v>1</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E31" s="13"/>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="30" t="s">
         <v>175</v>
       </c>
       <c r="G31" s="13"/>
@@ -2183,7 +2218,7 @@
       <c r="J31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K31" s="34" t="s">
+      <c r="K31" s="31" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2197,11 +2232,11 @@
       <c r="C32" s="13">
         <v>1</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="13"/>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="30" t="s">
         <v>96</v>
       </c>
       <c r="G32" s="13"/>
@@ -2214,7 +2249,7 @@
       <c r="J32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K32" s="34" t="s">
+      <c r="K32" s="31" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2228,11 +2263,11 @@
       <c r="C33" s="13">
         <v>1</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E33" s="13"/>
-      <c r="F33" s="33" t="s">
+      <c r="F33" s="30" t="s">
         <v>176</v>
       </c>
       <c r="G33" s="13"/>
@@ -2245,7 +2280,7 @@
       <c r="J33" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K33" s="35" t="s">
+      <c r="K33" s="32" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2259,11 +2294,11 @@
       <c r="C34" s="13">
         <v>1</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E34" s="13"/>
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="30" t="s">
         <v>176</v>
       </c>
       <c r="G34" s="13"/>
@@ -2276,7 +2311,7 @@
       <c r="J34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="34" t="s">
+      <c r="K34" s="31" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2290,11 +2325,11 @@
       <c r="C35" s="13">
         <v>1</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E35" s="13"/>
-      <c r="F35" s="33" t="s">
+      <c r="F35" s="30" t="s">
         <v>176</v>
       </c>
       <c r="G35" s="13"/>
@@ -2307,7 +2342,7 @@
       <c r="J35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="34" t="s">
+      <c r="K35" s="31" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2321,11 +2356,11 @@
       <c r="C36" s="13">
         <v>1</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E36" s="13"/>
-      <c r="F36" s="33" t="s">
+      <c r="F36" s="30" t="s">
         <v>178</v>
       </c>
       <c r="G36" s="13"/>
@@ -2338,7 +2373,7 @@
       <c r="J36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K36" s="34" t="s">
+      <c r="K36" s="31" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2352,11 +2387,11 @@
       <c r="C37" s="13">
         <v>2</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E37" s="13"/>
-      <c r="F37" s="33" t="s">
+      <c r="F37" s="30" t="s">
         <v>96</v>
       </c>
       <c r="G37" s="13"/>
@@ -2369,7 +2404,7 @@
       <c r="J37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K37" s="34" t="s">
+      <c r="K37" s="31" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2383,11 +2418,13 @@
       <c r="C38" s="13">
         <v>1</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E38" s="13"/>
-      <c r="F38" s="33"/>
+      <c r="F38" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G38" s="13"/>
       <c r="H38" s="15">
         <v>1.02</v>
@@ -2398,7 +2435,7 @@
       <c r="J38" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K38" s="34" t="s">
+      <c r="K38" s="31" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2409,12 +2446,16 @@
       <c r="B39" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="33" t="s">
+      <c r="C39" s="13">
+        <v>2</v>
+      </c>
+      <c r="D39" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E39" s="13"/>
-      <c r="F39" s="33"/>
+      <c r="F39" s="30" t="s">
+        <v>200</v>
+      </c>
       <c r="G39" s="13"/>
       <c r="H39" s="15">
         <v>1.02</v>
@@ -2425,1014 +2466,1227 @@
       <c r="J39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K39" s="37" t="s">
+      <c r="K39" s="32" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
+    <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="19">
+        <v>1</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" s="13">
+        <v>2</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>89</v>
+      </c>
       <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
+      <c r="F40" s="30" t="s">
+        <v>200</v>
+      </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="16"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="13" t="s">
+      <c r="H40" s="15">
+        <v>7.98</v>
+      </c>
+      <c r="I40" s="15">
+        <v>7.98</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="19">
+        <v>1</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C41" s="13">
+        <v>1</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="I41" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="19">
+        <v>1</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="13">
+        <v>1</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="15">
+        <v>1.23</v>
+      </c>
+      <c r="I42" s="15">
+        <v>1.23</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="19">
+        <v>1</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C43" s="13">
+        <v>1</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="15">
+        <v>3.89</v>
+      </c>
+      <c r="I43" s="15">
+        <v>3.89</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
+        <v>1</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="13">
+        <v>1</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G44" s="13"/>
+      <c r="H44" s="15">
+        <v>1.74</v>
+      </c>
+      <c r="I44" s="15">
+        <v>1.74</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="19">
+        <v>1</v>
+      </c>
+      <c r="B45" s="16">
+        <v>560112110224</v>
+      </c>
+      <c r="C45" s="13">
+        <v>1</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G45" s="13"/>
+      <c r="H45" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="I45" s="15"/>
+      <c r="J45" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="19">
+        <v>1</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="13">
+        <v>10</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="15">
+        <v>13.1</v>
+      </c>
+      <c r="I46" s="15">
+        <v>13.1</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="32"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="16"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+      <c r="B48" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15">
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13" t="s">
+      <c r="J48" s="13"/>
+      <c r="K48" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="13" t="s">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+      <c r="B49" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15">
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13" t="s">
+      <c r="J49" s="13"/>
+      <c r="K49" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="13" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+      <c r="B50" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15">
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13" t="s">
+      <c r="J50" s="13"/>
+      <c r="K50" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="13" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
+      <c r="B51" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15">
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="13" t="s">
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="22"/>
+      <c r="B52" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15">
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-    </row>
-    <row r="46" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+    </row>
+    <row r="53" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H54" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K54" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
+    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-    </row>
-    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="17">
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+    </row>
+    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="17">
         <v>3</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B56" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="13">
+      <c r="C56" s="13">
         <v>4</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D56" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="23" t="s">
+      <c r="E56" s="20"/>
+      <c r="F56" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="G49" s="13" t="s">
+      <c r="G56" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="H49" s="15">
+      <c r="H56" s="15">
         <v>224.4</v>
       </c>
-      <c r="I49" s="15">
-        <f>C49*H49</f>
+      <c r="I56" s="15">
+        <f>C56*H56</f>
         <v>897.6</v>
       </c>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13" t="s">
+      <c r="J56" s="13"/>
+      <c r="K56" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="12">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="12">
         <v>2</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B57" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="13">
+      <c r="C57" s="13">
         <v>4</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D57" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E57" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F57" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G50" s="13" t="s">
+      <c r="G57" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H57" s="15">
         <v>198.352</v>
       </c>
-      <c r="I50" s="15">
-        <f>C50*H50</f>
+      <c r="I57" s="15">
+        <f>C57*H57</f>
         <v>793.40800000000002</v>
       </c>
-      <c r="J50" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K50" s="13" t="s">
+      <c r="J57" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K57" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
-        <v>1</v>
-      </c>
-      <c r="B51" s="13" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="19">
+        <v>1</v>
+      </c>
+      <c r="B58" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="13">
+      <c r="C58" s="13">
         <v>24</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D58" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14" t="s">
+      <c r="E58" s="13"/>
+      <c r="F58" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G51" s="13" t="s">
+      <c r="G58" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H58" s="15">
         <v>309</v>
       </c>
-      <c r="I51" s="15">
-        <f>C51*H51</f>
+      <c r="I58" s="15">
+        <f>C58*H58</f>
         <v>7416</v>
       </c>
-      <c r="J51" s="13" t="s">
+      <c r="J58" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K51" s="13" t="s">
+      <c r="K58" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+    <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="19">
-        <v>1</v>
-      </c>
-      <c r="B53" s="13" t="s">
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="19">
+        <v>1</v>
+      </c>
+      <c r="B60" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="13">
+      <c r="C60" s="13">
         <v>10</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D60" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14" t="s">
+      <c r="E60" s="13"/>
+      <c r="F60" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G60" s="13">
         <v>2536030320001</v>
       </c>
-      <c r="H53" s="15">
+      <c r="H60" s="15">
         <v>0</v>
       </c>
-      <c r="I53" s="15">
-        <f>C53*H53</f>
+      <c r="I60" s="15">
+        <f>C60*H60</f>
         <v>0</v>
       </c>
-      <c r="J53" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K53" s="13" t="s">
+      <c r="J60" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
+    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A61" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="19">
-        <v>1</v>
-      </c>
-      <c r="B55" s="13" t="s">
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="19">
+        <v>1</v>
+      </c>
+      <c r="B62" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C55" s="13">
-        <v>1</v>
-      </c>
-      <c r="D55" s="14" t="s">
+      <c r="C62" s="13">
+        <v>1</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E62" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F62" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G55" s="13"/>
-      <c r="H55" s="15">
+      <c r="G62" s="13"/>
+      <c r="H62" s="15">
         <v>369</v>
       </c>
-      <c r="I55" s="15">
-        <f>H55*C55</f>
+      <c r="I62" s="15">
+        <f>H62*C62</f>
         <v>369</v>
       </c>
-      <c r="J55" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K55" s="24" t="str">
+      <c r="J62" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="24" t="str">
         <f>"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B20</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="17">
         <v>3</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B63" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="13">
-        <v>1</v>
-      </c>
-      <c r="D56" s="14" t="s">
+      <c r="C63" s="13">
+        <v>1</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E63" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="F63" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G56" s="13" t="s">
+      <c r="G63" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="H56" s="15">
+      <c r="H63" s="15">
         <v>605.13</v>
       </c>
-      <c r="I56" s="15">
-        <f>C56*H56</f>
+      <c r="I63" s="15">
+        <f>C63*H63</f>
         <v>605.13</v>
       </c>
-      <c r="J56" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K56" s="13" t="s">
+      <c r="J63" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A64" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
-    </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="19">
-        <v>1</v>
-      </c>
-      <c r="B58" s="13" t="s">
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="35"/>
+    </row>
+    <row r="65" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="19">
+        <v>1</v>
+      </c>
+      <c r="B65" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="13">
-        <v>1</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C65" s="13">
+        <v>1</v>
+      </c>
+      <c r="D65" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="13">
+      <c r="E65" s="13">
         <v>41015028</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F65" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G58" s="13"/>
-      <c r="H58" s="15">
+      <c r="G65" s="13"/>
+      <c r="H65" s="15">
         <v>99</v>
       </c>
-      <c r="I58" s="15">
-        <f>H58*C58</f>
+      <c r="I65" s="15">
+        <f>H65*C65</f>
         <v>99</v>
       </c>
-      <c r="J58" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K58" s="13" t="s">
+      <c r="J65" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
+    <row r="66" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A66" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="31"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="3" t="s">
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="34"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F67" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H67" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="I67" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J60" s="3" t="s">
+      <c r="J67" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K60" s="3" t="s">
+      <c r="K67" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="19">
-        <v>1</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C67" s="13">
-        <v>4</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E67" s="13">
-        <v>41019265</v>
-      </c>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="15">
-        <v>18</v>
-      </c>
-      <c r="I67" s="15">
-        <f>C67*H67</f>
-        <v>72</v>
-      </c>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="30"/>
-    </row>
-    <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="35"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="35"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
       <c r="B69" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C69" s="13">
-        <v>3</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E69" s="25">
-        <v>173010335</v>
-      </c>
-      <c r="F69" s="13" t="s">
-        <v>119</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
       <c r="G69" s="13"/>
-      <c r="H69" s="15">
-        <v>0</v>
-      </c>
+      <c r="H69" s="15"/>
       <c r="I69" s="15"/>
-      <c r="J69" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K69" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
       <c r="B70" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="13">
-        <v>3</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E70" s="25">
-        <v>173010542</v>
-      </c>
-      <c r="F70" s="13" t="s">
-        <v>119</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
       <c r="G70" s="13"/>
-      <c r="H70" s="15">
-        <v>0</v>
-      </c>
+      <c r="H70" s="15"/>
       <c r="I70" s="15"/>
-      <c r="J70" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="J70" s="13"/>
       <c r="K70" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
       <c r="B71" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C71" s="13">
-        <v>3</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E71" s="13">
-        <v>173011235</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>119</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
       <c r="G71" s="13"/>
-      <c r="H71" s="15">
-        <v>0</v>
-      </c>
+      <c r="H71" s="15"/>
       <c r="I71" s="15"/>
-      <c r="J71" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="J71" s="13"/>
       <c r="K71" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="22"/>
       <c r="B72" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="22"/>
+      <c r="B73" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="19">
+        <v>1</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" s="13">
+        <v>4</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" s="13">
+        <v>41019265</v>
+      </c>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="15">
+        <v>18</v>
+      </c>
+      <c r="I74" s="15">
+        <f>C74*H74</f>
+        <v>72</v>
+      </c>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A75" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="35"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="35"/>
+      <c r="J75" s="35"/>
+      <c r="K75" s="35"/>
+    </row>
+    <row r="76" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="22"/>
+      <c r="B76" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="13">
+        <v>3</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E76" s="25">
+        <v>173010335</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G76" s="13"/>
+      <c r="H76" s="15">
+        <v>0</v>
+      </c>
+      <c r="I76" s="15"/>
+      <c r="J76" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K76" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="22"/>
+      <c r="B77" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77" s="13">
+        <v>3</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E77" s="25">
+        <v>173010542</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G77" s="13"/>
+      <c r="H77" s="15">
+        <v>0</v>
+      </c>
+      <c r="I77" s="15"/>
+      <c r="J77" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A78" s="22"/>
+      <c r="B78" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="13">
+        <v>3</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E78" s="13">
+        <v>173011235</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G78" s="13"/>
+      <c r="H78" s="15">
+        <v>0</v>
+      </c>
+      <c r="I78" s="15"/>
+      <c r="J78" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K78" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A79" s="22"/>
+      <c r="B79" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C72" s="13">
+      <c r="C79" s="13">
         <v>3</v>
       </c>
-      <c r="D72" s="20" t="s">
+      <c r="D79" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E79" s="25">
         <v>173011535</v>
       </c>
-      <c r="F72" s="13" t="s">
+      <c r="F79" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G72" s="13"/>
-      <c r="H72" s="15">
+      <c r="G79" s="13"/>
+      <c r="H79" s="15">
         <v>0</v>
       </c>
-      <c r="I72" s="15"/>
-      <c r="J72" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K72" s="13" t="s">
+      <c r="I79" s="15"/>
+      <c r="J79" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K79" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A73" s="31" t="s">
+    <row r="80" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A80" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="31"/>
-      <c r="J73" s="31"/>
-      <c r="K73" s="31"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="3" t="s">
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="34"/>
+      <c r="J80" s="34"/>
+      <c r="K80" s="34"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F81" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G81" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H81" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I74" s="4" t="s">
+      <c r="I81" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J74" s="3" t="s">
+      <c r="J81" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K74" s="3" t="s">
+      <c r="K81" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
+    <row r="82" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A82" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="19">
-        <v>1</v>
-      </c>
-      <c r="B76" s="13" t="s">
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="35"/>
+      <c r="J82" s="35"/>
+      <c r="K82" s="35"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="19">
+        <v>1</v>
+      </c>
+      <c r="B83" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C76" s="13">
+      <c r="C83" s="13">
         <v>6</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D83" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E76" s="13"/>
-      <c r="F76" s="14" t="s">
+      <c r="E83" s="13"/>
+      <c r="F83" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G76" s="13" t="s">
+      <c r="G83" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="H76" s="15">
+      <c r="H83" s="15">
         <v>262.83</v>
       </c>
-      <c r="I76" s="15">
-        <f>C76*H76</f>
+      <c r="I83" s="15">
+        <f>C83*H83</f>
         <v>1576.98</v>
       </c>
-      <c r="J76" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="13" t="s">
+      <c r="J83" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K83" s="13" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
-      <c r="B77" s="16" t="s">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="12"/>
+      <c r="B84" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C77" s="13">
-        <v>1</v>
-      </c>
-      <c r="D77" s="14" t="s">
+      <c r="C84" s="13">
+        <v>1</v>
+      </c>
+      <c r="D84" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="E77" s="13">
+      <c r="E84" s="13">
         <v>5901259432770</v>
       </c>
-      <c r="F77" s="14" t="s">
+      <c r="F84" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="G77" s="13" t="s">
+      <c r="G84" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="H77" s="15">
+      <c r="H84" s="15">
         <v>237</v>
       </c>
-      <c r="I77" s="15">
-        <f>C77*H77</f>
+      <c r="I84" s="15">
+        <f>C84*H84</f>
         <v>237</v>
       </c>
-      <c r="J77" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K77" s="13"/>
-    </row>
-    <row r="81" spans="2:7" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B81" s="26" t="s">
+      <c r="J84" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K84" s="13"/>
+    </row>
+    <row r="88" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B88" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="C81" s="27">
-        <f>SUM(I4,I9,I13,I18,I19,I22,I23,I25,I28,I51,I55,I58,I67)</f>
+      <c r="C88" s="27">
+        <f>SUM(I4,I9,I13,I18,I19,I22,I23,I25,I28,I58,I62,I65,I74)</f>
         <v>14365.224999999999</v>
       </c>
-      <c r="E81" s="32" t="s">
+      <c r="E88" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F81" s="32"/>
-      <c r="G81" s="28" t="s">
+      <c r="F88" s="36"/>
+      <c r="G88" s="28" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="B82" s="29" t="s">
+    <row r="89" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B89" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="E82" s="13" t="s">
+      <c r="E89" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="F82" s="19"/>
-      <c r="G82" s="13" t="s">
+      <c r="F89" s="19"/>
+      <c r="G89" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B83" s="13" t="s">
+    <row r="90" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B90" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E83" s="13" t="s">
+      <c r="E90" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F83" s="12"/>
-      <c r="G83" s="13"/>
-    </row>
-    <row r="84" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B84" s="13" t="s">
+      <c r="F90" s="12"/>
+      <c r="G90" s="13"/>
+    </row>
+    <row r="91" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B91" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E84" s="13" t="s">
+      <c r="E91" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="F84" s="17"/>
-      <c r="G84" s="13"/>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="13" t="s">
+      <c r="F91" s="17"/>
+      <c r="G91" s="13"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E85" s="13" t="s">
+      <c r="E92" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F85" s="22"/>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="13" t="s">
+      <c r="F92" s="22"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="13" t="s">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B94" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="13" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B95" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="13" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B96" s="13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90"/>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="24"/>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="24"/>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="24"/>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="24"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="24"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A80:K80"/>
+    <mergeCell ref="A82:K82"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A61:K61"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A55:K55"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="A16:K16"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="A73:K73"/>
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A61:K61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3465,27 +3719,27 @@
     <hyperlink ref="D26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="D28" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="F28" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D49" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F49" r:id="rId32" location="documents" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F50" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D51" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F51" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D53" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="F53" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D55" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="D56" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F56" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D58" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D67" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D69" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D70" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D71" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D72" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="D76" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="F76" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D77" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="F77" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="D56" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F56" r:id="rId32" location="documents" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D57" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F57" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D58" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F58" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D60" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F60" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D62" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D63" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F63" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D65" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D74" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D76" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D77" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D78" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D79" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D83" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F83" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D84" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F84" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
     <hyperlink ref="D29" r:id="rId52" xr:uid="{876E345E-1D94-4A3A-B802-012FDED57481}"/>
     <hyperlink ref="F29" r:id="rId53" xr:uid="{628119BE-F2D7-4277-A29F-A0FFDCCE110D}"/>
     <hyperlink ref="D30" r:id="rId54" xr:uid="{BD7440CF-9727-473C-A25D-FB5A217BDA81}"/>
@@ -3506,13 +3760,29 @@
     <hyperlink ref="F37" r:id="rId69" xr:uid="{89F13473-EADE-4FC1-9A68-F9AC21EAA78B}"/>
     <hyperlink ref="D38" r:id="rId70" xr:uid="{11380CE5-128C-470B-B728-27DF70A3633B}"/>
     <hyperlink ref="D39" r:id="rId71" xr:uid="{4336C976-5B02-48FA-B06D-E8DE994D7146}"/>
+    <hyperlink ref="D40" r:id="rId72" xr:uid="{F45A07D9-FF61-4159-9344-7B60D6017DAB}"/>
+    <hyperlink ref="D41" r:id="rId73" xr:uid="{C989FA4D-5F97-4828-A5A1-0F9998475A2F}"/>
+    <hyperlink ref="F41" r:id="rId74" xr:uid="{79C0125F-0FC4-4F40-B62E-10A976B6218F}"/>
+    <hyperlink ref="F40" r:id="rId75" xr:uid="{2783F514-150F-4159-AF66-F6CEA642DDB8}"/>
+    <hyperlink ref="F39" r:id="rId76" xr:uid="{D97AD0D6-479F-4C4F-B07C-18D6EE480DF2}"/>
+    <hyperlink ref="F38" r:id="rId77" xr:uid="{0E9260A0-94A6-4210-A568-8EB93C7C6CED}"/>
+    <hyperlink ref="D42" r:id="rId78" xr:uid="{3E6E462A-DA80-4AEB-B565-184AA045552E}"/>
+    <hyperlink ref="F42" r:id="rId79" xr:uid="{EEC71709-7132-40C9-877F-68EC24D23C0A}"/>
+    <hyperlink ref="D43" r:id="rId80" xr:uid="{0084EAC1-A830-4506-AEC6-09D7F23FF463}"/>
+    <hyperlink ref="F43" r:id="rId81" xr:uid="{9EBBD898-2ACE-49CD-A261-F0C85F9044CD}"/>
+    <hyperlink ref="D44" r:id="rId82" xr:uid="{66AD4326-F47A-4042-AE5C-0707B089A923}"/>
+    <hyperlink ref="F44" r:id="rId83" xr:uid="{3262FC35-5C88-43D6-B59B-BDACF37EF0B6}"/>
+    <hyperlink ref="D45" r:id="rId84" xr:uid="{7CDF5B9E-88E1-420B-BE63-3AC061A6D064}"/>
+    <hyperlink ref="F45" r:id="rId85" xr:uid="{9CC6F8BC-C722-484B-A21B-AFCDAC8A3796}"/>
+    <hyperlink ref="D46" r:id="rId86" xr:uid="{5271594F-B797-424D-AEBC-E8A590480170}"/>
+    <hyperlink ref="F46" r:id="rId87" xr:uid="{5C3D4144-78C7-4B49-BEF4-D46959CA2EE5}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId72"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId88"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId73"/>
+  <legacyDrawing r:id="rId89"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some of the kicker components to BOM.xlsx
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="175">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t xml:space="preserve">Output diodes, SMD, T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420VXG180MEFCSN25X35</t>
   </si>
   <si>
     <t xml:space="preserve">Sensors</t>
@@ -745,7 +748,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -817,18 +820,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="10"/>
       <color theme="10"/>
@@ -862,6 +853,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -966,7 +962,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1063,11 +1059,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1075,11 +1067,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1087,15 +1075,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1297,8 +1285,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K32" activeCellId="0" sqref="K32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2123,13 +2111,13 @@
       <c r="C29" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="16" t="s">
         <v>89</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="25" t="s">
+      <c r="F29" s="16" t="s">
         <v>91</v>
       </c>
       <c r="G29" s="15" t="s">
@@ -2150,20 +2138,22 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26"/>
+      <c r="A30" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B30" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="25" t="s">
+      <c r="F30" s="16" t="s">
         <v>95</v>
       </c>
       <c r="G30" s="15" t="s">
@@ -2184,20 +2174,22 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26"/>
+      <c r="A31" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="B31" s="15" t="s">
         <v>97</v>
       </c>
       <c r="C31" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="16" t="s">
         <v>89</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="16" t="s">
         <v>99</v>
       </c>
       <c r="G31" s="15" t="s">
@@ -2206,7 +2198,7 @@
       <c r="H31" s="17" t="n">
         <v>4.09</v>
       </c>
-      <c r="I31" s="27" t="n">
+      <c r="I31" s="17" t="n">
         <f aca="false">C31*H31</f>
         <v>8.18</v>
       </c>
@@ -2218,9 +2210,13 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="15" t="n">
+        <v>10</v>
+      </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
@@ -2231,7 +2227,7 @@
       <c r="K32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -2245,7 +2241,7 @@
     </row>
     <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2295,7 +2291,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -2313,20 +2309,20 @@
         <v>1</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D37" s="28" t="s">
-        <v>104</v>
+      <c r="D37" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="E37" s="22"/>
-      <c r="F37" s="28" t="s">
-        <v>105</v>
+      <c r="F37" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H37" s="17" t="n">
         <v>224.4</v>
@@ -2337,7 +2333,7 @@
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C38" s="15" t="n">
         <v>24</v>
@@ -2355,10 +2351,10 @@
       </c>
       <c r="E38" s="15"/>
       <c r="F38" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H38" s="17" t="n">
         <v>309</v>
@@ -2368,10 +2364,10 @@
         <v>7416</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,7 +2375,7 @@
         <v>3</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C39" s="15" t="n">
         <v>4</v>
@@ -2388,13 +2384,13 @@
         <v>42</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H39" s="17" t="n">
         <v>198.352</v>
@@ -2407,12 +2403,12 @@
         <v>16</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2430,17 +2426,17 @@
         <v>1</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C41" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G41" s="15" t="n">
         <v>2536030320001</v>
@@ -2456,12 +2452,12 @@
         <v>16</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2479,7 +2475,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" s="15" t="n">
         <v>1</v>
@@ -2488,7 +2484,7 @@
         <v>60</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>62</v>
@@ -2504,7 +2500,7 @@
       <c r="J43" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K43" s="29" t="str">
+      <c r="K43" s="27" t="str">
         <f aca="false">"Needs to be ordered with " &amp; BOM!B17 &amp; "or " &amp; BOM!B20</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
@@ -2514,7 +2510,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C44" s="15" t="n">
         <v>1</v>
@@ -2523,13 +2519,13 @@
         <v>42</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H44" s="17" t="n">
         <v>605.13</v>
@@ -2542,12 +2538,12 @@
         <v>16</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2565,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C46" s="15" t="n">
         <v>1</v>
@@ -2577,7 +2573,7 @@
         <v>41015028</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="17" t="n">
@@ -2591,12 +2587,12 @@
         <v>16</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2656,9 +2652,9 @@
       <c r="K49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="26"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -2671,9 +2667,9 @@
       <c r="K50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
@@ -2684,13 +2680,13 @@
       <c r="I51" s="17"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="26"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
@@ -2701,13 +2697,13 @@
       <c r="I52" s="17"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="26"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -2718,13 +2714,13 @@
       <c r="I53" s="17"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="26"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -2735,7 +2731,7 @@
       <c r="I54" s="17"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2743,13 +2739,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C55" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E55" s="15" t="n">
         <v>41019265</v>
@@ -2765,12 +2761,12 @@
       </c>
       <c r="J55" s="15"/>
       <c r="K55" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -2784,21 +2780,21 @@
       <c r="K56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="26"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C57" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="E57" s="30" t="n">
+        <v>120</v>
+      </c>
+      <c r="E57" s="28" t="n">
         <v>173010335</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="17" t="n">
@@ -2809,25 +2805,25 @@
         <v>16</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" s="30" t="n">
+        <v>120</v>
+      </c>
+      <c r="E58" s="28" t="n">
         <v>173010542</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G58" s="15"/>
       <c r="H58" s="17" t="n">
@@ -2838,25 +2834,25 @@
         <v>16</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="26"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E59" s="15" t="n">
         <v>173011235</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="17" t="n">
@@ -2867,25 +2863,25 @@
         <v>16</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="26"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C60" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" s="30" t="n">
+        <v>120</v>
+      </c>
+      <c r="E60" s="28" t="n">
         <v>173011535</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="17" t="n">
@@ -2896,12 +2892,12 @@
         <v>16</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2949,7 +2945,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -2967,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C64" s="15" t="n">
         <v>6</v>
@@ -2977,10 +2973,10 @@
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H64" s="17" t="n">
         <v>262.83</v>
@@ -2993,28 +2989,28 @@
         <v>16</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="14"/>
       <c r="B65" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C65" s="15" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E65" s="15" t="n">
         <v>5901259432770</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H65" s="17" t="n">
         <v>237</v>
@@ -3029,90 +3025,90 @@
       <c r="K65" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C69" s="32" t="n">
+      <c r="B69" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="30" t="n">
         <f aca="false">SUM(I4,I9,I13,I17,I18,I22,I23,I25,I28,I38,I43,I46,I55)</f>
         <v>14218.3</v>
       </c>
-      <c r="E69" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="F69" s="33"/>
-      <c r="G69" s="34" t="s">
+      <c r="E69" s="31" t="s">
         <v>162</v>
       </c>
+      <c r="F69" s="31"/>
+      <c r="G69" s="32" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="35" t="s">
-        <v>163</v>
+      <c r="B70" s="33" t="s">
+        <v>164</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="F73" s="26"/>
+        <v>171</v>
+      </c>
+      <c r="F73" s="25"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="15" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="29"/>
+      <c r="B79" s="27"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="29"/>
+      <c r="B80" s="27"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="29"/>
+      <c r="B81" s="27"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
BOM.xlsx: Changed the ranking of the ESC components
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -962,7 +962,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1049,6 +1049,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1285,8 +1289,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1566,8 +1570,8 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>1</v>
+      <c r="A11" s="22" t="n">
+        <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>36</v>
@@ -1602,8 +1606,8 @@
       </c>
     </row>
     <row r="12" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
-        <v>1</v>
+      <c r="A12" s="22" t="n">
+        <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>41</v>
@@ -1672,8 +1676,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="n">
-        <v>2</v>
+      <c r="A14" s="19" t="n">
+        <v>3</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>51</v>
@@ -1705,7 +1709,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>55</v>
@@ -1861,7 +1865,7 @@
       <c r="C20" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="23" t="s">
         <v>60</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -1901,14 +1905,14 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="15" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="23" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -1935,14 +1939,14 @@
       </c>
     </row>
     <row r="23" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="23" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -2105,7 +2109,7 @@
       <c r="A29" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="25" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="15" t="n">
@@ -2210,7 +2214,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="15" t="s">
         <v>101</v>
       </c>
@@ -2227,7 +2231,7 @@
       <c r="K32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -2314,11 +2318,11 @@
       <c r="C37" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="26" t="s">
+      <c r="E37" s="23"/>
+      <c r="F37" s="27" t="s">
         <v>106</v>
       </c>
       <c r="G37" s="15" t="s">
@@ -2500,7 +2504,7 @@
       <c r="J43" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K43" s="27" t="str">
+      <c r="K43" s="28" t="str">
         <f aca="false">"Needs to be ordered with " &amp; BOM!B17 &amp; "or " &amp; BOM!B20</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
@@ -2566,7 +2570,7 @@
       <c r="C46" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="23" t="s">
         <v>60</v>
       </c>
       <c r="E46" s="15" t="n">
@@ -2652,7 +2656,7 @@
       <c r="K49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="15" t="s">
         <v>136</v>
       </c>
@@ -2667,7 +2671,7 @@
       <c r="K50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="25"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="15" t="s">
         <v>137</v>
       </c>
@@ -2684,7 +2688,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="25"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="15" t="s">
         <v>139</v>
       </c>
@@ -2701,7 +2705,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="15" t="s">
         <v>140</v>
       </c>
@@ -2718,7 +2722,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="25"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="15" t="s">
         <v>141</v>
       </c>
@@ -2780,17 +2784,17 @@
       <c r="K56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C57" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="28" t="n">
+      <c r="E57" s="29" t="n">
         <v>173010335</v>
       </c>
       <c r="F57" s="15" t="s">
@@ -2809,17 +2813,17 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="15" t="s">
         <v>148</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="28" t="n">
+      <c r="E58" s="29" t="n">
         <v>173010542</v>
       </c>
       <c r="F58" s="15" t="s">
@@ -2838,14 +2842,14 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="15" t="s">
         <v>149</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D59" s="23" t="s">
         <v>120</v>
       </c>
       <c r="E59" s="15" t="n">
@@ -2867,17 +2871,17 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="25"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="15" t="s">
         <v>150</v>
       </c>
       <c r="C60" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="E60" s="28" t="n">
+      <c r="E60" s="29" t="n">
         <v>173011535</v>
       </c>
       <c r="F60" s="15" t="s">
@@ -3025,23 +3029,23 @@
       <c r="K65" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C69" s="30" t="n">
-        <f aca="false">SUM(I4,I9,I13,I17,I18,I22,I23,I25,I28,I38,I43,I46,I55)</f>
-        <v>14218.3</v>
-      </c>
-      <c r="E69" s="31" t="s">
+      <c r="C69" s="31" t="n">
+        <f aca="false">SUM(I4,I9,I13,I17,I18,I22,I23,I25,I28,I37,I43,I46,I55)</f>
+        <v>7699.9</v>
+      </c>
+      <c r="E69" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="F69" s="31"/>
-      <c r="G69" s="32" t="s">
+      <c r="F69" s="32"/>
+      <c r="G69" s="33" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="33" t="s">
+      <c r="B70" s="34" t="s">
         <v>164</v>
       </c>
       <c r="E70" s="15" t="s">
@@ -3079,7 +3083,7 @@
       <c r="E73" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="F73" s="25"/>
+      <c r="F73" s="26"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="15" t="s">
@@ -3102,13 +3106,13 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="27"/>
+      <c r="B79" s="28"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="27"/>
+      <c r="B80" s="28"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="27"/>
+      <c r="B81" s="28"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
BOM.xlsx: Added RGB color sensor that UdeA uses
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="201">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -294,26 +294,7 @@
     <t xml:space="preserve">STMicroelectronics</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Datasheet </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The ESC is compatible with sensorless BLDC motors and will work similarly to the UdeAs ESC. </t>
-    </r>
+    <t xml:space="preserve">Datasheet The ESC is compatible with sensorless BLDC motors and will work similarly to the UdeAs ESC. </t>
   </si>
   <si>
     <t xml:space="preserve">Aerostar 30A RVS G2 32bit ESC</t>
@@ -624,6 +605,15 @@
   </si>
   <si>
     <t xml:space="preserve">Break beam to detect if a ball is close (within a few mm) to the dribbler.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GY-9960-3.3 APDS-9960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proto Supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB sensor chosen by UdeA for ball detection.</t>
   </si>
   <si>
     <t xml:space="preserve">3D CAD and Mechanical</t>
@@ -836,7 +826,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -889,13 +879,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1053,11 +1036,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1154,15 +1137,11 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1170,7 +1149,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1178,11 +1157,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1190,19 +1169,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1402,10 +1381,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1488,7 +1467,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" s="13" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>1</v>
       </c>
@@ -1520,7 +1499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="true" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
         <v>18</v>
       </c>
@@ -1552,7 +1531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="57.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="n">
         <v>2</v>
       </c>
@@ -1822,7 +1801,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="n">
         <v>3</v>
       </c>
@@ -1917,7 +1896,7 @@
       <c r="E18" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="17" t="s">
         <v>67</v>
       </c>
       <c r="G18" s="16"/>
@@ -1936,7 +1915,7 @@
         <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
         <v>1</v>
       </c>
@@ -1973,7 +1952,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1988,7 +1967,7 @@
       <c r="E20" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="17" t="s">
         <v>73</v>
       </c>
       <c r="G20" s="16" t="s">
@@ -2018,7 +1997,7 @@
       <c r="C21" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>65</v>
       </c>
       <c r="E21" s="16" t="s">
@@ -2058,14 +2037,14 @@
       <c r="K22" s="6"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C23" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -2092,14 +2071,14 @@
       </c>
     </row>
     <row r="24" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="16" t="s">
         <v>83</v>
       </c>
       <c r="C24" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -2262,7 +2241,7 @@
       <c r="A30" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>95</v>
       </c>
       <c r="C30" s="16" t="n">
@@ -2367,7 +2346,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="16" t="s">
         <v>108</v>
       </c>
@@ -2384,7 +2363,7 @@
       <c r="K33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
@@ -2461,7 +2440,7 @@
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="n">
         <v>1</v>
       </c>
@@ -2471,11 +2450,11 @@
       <c r="C38" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="30" t="s">
+      <c r="E38" s="25"/>
+      <c r="F38" s="29" t="s">
         <v>113</v>
       </c>
       <c r="G38" s="16" t="s">
@@ -2493,7 +2472,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
         <v>18</v>
       </c>
@@ -2503,13 +2482,13 @@
       <c r="C39" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="29" t="s">
         <v>118</v>
       </c>
       <c r="G39" s="16" t="s">
@@ -2681,7 +2660,7 @@
       <c r="E45" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="17" t="s">
         <v>67</v>
       </c>
       <c r="G45" s="16"/>
@@ -2695,7 +2674,7 @@
       <c r="J45" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K45" s="32" t="str">
+      <c r="K45" s="31" t="str">
         <f aca="false">"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B21</f>
         <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
@@ -2716,7 +2695,7 @@
       <c r="E46" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F46" s="17" t="s">
         <v>142</v>
       </c>
       <c r="G46" s="16" t="s">
@@ -2732,7 +2711,7 @@
       <c r="J46" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="32" t="s">
+      <c r="K46" s="31" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2746,13 +2725,13 @@
       <c r="C47" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="D47" s="17" t="s">
         <v>146</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="F47" s="33" t="s">
+      <c r="F47" s="32" t="s">
         <v>142</v>
       </c>
       <c r="G47" s="16" t="s">
@@ -2768,7 +2747,7 @@
       <c r="J47" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K47" s="32" t="s">
+      <c r="K47" s="31" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2833,7 +2812,7 @@
       <c r="C50" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D50" s="26" t="s">
+      <c r="D50" s="25" t="s">
         <v>65</v>
       </c>
       <c r="E50" s="16" t="n">
@@ -2857,86 +2836,100 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="16"/>
-      <c r="B52" s="4" t="s">
+      <c r="C51" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="18" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="I51" s="18" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="16"/>
+      <c r="B53" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F53" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G53" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H53" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="I53" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="J53" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="29"/>
-      <c r="B54" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="29"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="16" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
@@ -2946,14 +2939,12 @@
       <c r="H55" s="18"/>
       <c r="I55" s="18"/>
       <c r="J55" s="16"/>
-      <c r="K55" s="16" t="s">
-        <v>161</v>
-      </c>
+      <c r="K55" s="16"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="29"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
@@ -2964,13 +2955,13 @@
       <c r="I56" s="18"/>
       <c r="J56" s="16"/>
       <c r="K56" s="16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="29"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="16" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
@@ -2981,13 +2972,13 @@
       <c r="I57" s="18"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="29"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="16" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
@@ -2998,96 +2989,84 @@
       <c r="I58" s="18"/>
       <c r="J58" s="16"/>
       <c r="K58" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="22" t="n">
-        <v>1</v>
-      </c>
+      <c r="A59" s="28"/>
       <c r="B59" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C59" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D59" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E59" s="16" t="n">
-        <v>41019265</v>
-      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
-      <c r="H59" s="18" t="n">
-        <v>18</v>
-      </c>
-      <c r="I59" s="18" t="n">
-        <f aca="false">C59*H59</f>
-        <v>72</v>
-      </c>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
       <c r="J59" s="16"/>
       <c r="K59" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="29"/>
-      <c r="B61" s="16" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="D61" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="E61" s="34" t="n">
-        <v>173010335</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G61" s="16"/>
-      <c r="H61" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="18"/>
-      <c r="J61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K61" s="16" t="s">
+      <c r="C60" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" s="17" t="s">
         <v>170</v>
       </c>
+      <c r="E60" s="16" t="n">
+        <v>41019265</v>
+      </c>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="I60" s="18" t="n">
+        <f aca="false">C60*H60</f>
+        <v>72</v>
+      </c>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="29"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C62" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D62" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="E62" s="34" t="n">
-        <v>173010542</v>
+      <c r="E62" s="33" t="n">
+        <v>173010335</v>
       </c>
       <c r="F62" s="16" t="s">
         <v>134</v>
@@ -3101,22 +3080,22 @@
         <v>16</v>
       </c>
       <c r="K62" s="16" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="29"/>
+      <c r="A63" s="28"/>
       <c r="B63" s="16" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C63" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D63" s="26" t="s">
+      <c r="D63" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="E63" s="16" t="n">
-        <v>173011235</v>
+      <c r="E63" s="33" t="n">
+        <v>173010542</v>
       </c>
       <c r="F63" s="16" t="s">
         <v>134</v>
@@ -3130,22 +3109,22 @@
         <v>16</v>
       </c>
       <c r="K63" s="16" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="29"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C64" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D64" s="26" t="s">
+      <c r="D64" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="34" t="n">
-        <v>173011535</v>
+      <c r="E64" s="16" t="n">
+        <v>173011235</v>
       </c>
       <c r="F64" s="16" t="s">
         <v>134</v>
@@ -3159,223 +3138,252 @@
         <v>16</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16"/>
-      <c r="B66" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="28"/>
+      <c r="B65" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C65" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E65" s="33" t="n">
+        <v>173011535</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G65" s="16"/>
+      <c r="H65" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16"/>
+      <c r="B67" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E67" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F67" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H67" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I67" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J66" s="4" t="s">
+      <c r="J67" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K66" s="4" t="s">
+      <c r="K67" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="C68" s="16" t="n">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D69" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E68" s="16"/>
-      <c r="F68" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="H68" s="18" t="n">
+      <c r="E69" s="16"/>
+      <c r="F69" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H69" s="18" t="n">
         <v>262.83</v>
-      </c>
-      <c r="I68" s="18" t="n">
-        <f aca="false">C68*H68</f>
-        <v>1576.98</v>
-      </c>
-      <c r="J68" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K68" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="15"/>
-      <c r="B69" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="C69" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="E69" s="16" t="n">
-        <v>5901259432770</v>
-      </c>
-      <c r="F69" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="H69" s="18" t="n">
-        <v>237</v>
       </c>
       <c r="I69" s="18" t="n">
         <f aca="false">C69*H69</f>
-        <v>237</v>
+        <v>1576.98</v>
       </c>
       <c r="J69" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K69" s="16"/>
-    </row>
-    <row r="73" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="35" t="s">
+      <c r="K69" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15"/>
+      <c r="B70" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C70" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C73" s="36" t="n">
-        <f aca="false">SUM(I4,I10,I14,I18,I19,I23,I24,I26,I29,I38,I45,I50,I59)</f>
+      <c r="E70" s="16" t="n">
+        <v>5901259432770</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="G70" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="H70" s="18" t="n">
+        <v>237</v>
+      </c>
+      <c r="I70" s="18" t="n">
+        <f aca="false">C70*H70</f>
+        <v>237</v>
+      </c>
+      <c r="J70" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="16"/>
+    </row>
+    <row r="74" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C74" s="35" t="n">
+        <f aca="false">SUM(I4,I10,I14,I18,I19,I23,I24,I26,I29,I38,I45,I50,I60)</f>
         <v>7699.9</v>
       </c>
-      <c r="E73" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="F73" s="37"/>
-      <c r="G73" s="38" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="F74" s="22"/>
-      <c r="G74" s="16" t="s">
+      <c r="F74" s="36"/>
+      <c r="G74" s="37" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="16" t="s">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="38" t="s">
         <v>190</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F75" s="15"/>
-      <c r="G75" s="16"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="16" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="16" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F76" s="20"/>
+        <v>194</v>
+      </c>
+      <c r="F76" s="15"/>
       <c r="G76" s="16"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="16" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="F77" s="29"/>
+        <v>195</v>
+      </c>
+      <c r="F77" s="20"/>
+      <c r="G77" s="16"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="16" t="s">
-        <v>195</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F78" s="28"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="16" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="16" t="s">
-        <v>131</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="32"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="16" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="32"/>
+      <c r="B84" s="31"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="32"/>
+      <c r="B85" s="31"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -3392,12 +3400,12 @@
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A44:K44"/>
     <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A60:K60"/>
-    <mergeCell ref="A65:K65"/>
-    <mergeCell ref="A67:K67"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A61:K61"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="E74:F74"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId2" display="Nanotec"/>
@@ -3414,7 +3422,7 @@
     <hyperlink ref="F13" r:id="rId13" display="Vishay"/>
     <hyperlink ref="D14" r:id="rId14" display="Mouser"/>
     <hyperlink ref="F14" r:id="rId15" display="STMicroelectronics"/>
-    <hyperlink ref="K14" r:id="rId16" display="Datasheet"/>
+    <hyperlink ref="K14" r:id="rId16" display="Datasheet The ESC is compatible with sensorless BLDC motors and will work similarly to the UdeAs ESC. "/>
     <hyperlink ref="D15" r:id="rId17" display="HobbyKing"/>
     <hyperlink ref="D16" r:id="rId18" display="HobbyKing"/>
     <hyperlink ref="D18" r:id="rId19" display="Electro:kit"/>
@@ -3456,15 +3464,16 @@
     <hyperlink ref="D48" r:id="rId55" display="Mouser"/>
     <hyperlink ref="F48" r:id="rId56" display="Texas Instruments"/>
     <hyperlink ref="D50" r:id="rId57" display="Electro:kit"/>
-    <hyperlink ref="D59" r:id="rId58" display="Electrokit"/>
-    <hyperlink ref="D61" r:id="rId59" display="Würth Electronic"/>
+    <hyperlink ref="D51" r:id="rId58" display="Proto Supplies"/>
+    <hyperlink ref="D60" r:id="rId59" display="Electrokit"/>
     <hyperlink ref="D62" r:id="rId60" display="Würth Electronic"/>
     <hyperlink ref="D63" r:id="rId61" display="Würth Electronic"/>
     <hyperlink ref="D64" r:id="rId62" display="Würth Electronic"/>
-    <hyperlink ref="D68" r:id="rId63" display="Farnell"/>
-    <hyperlink ref="F68" r:id="rId64" display="LEDEX"/>
-    <hyperlink ref="D69" r:id="rId65" display="Autodoc"/>
-    <hyperlink ref="F69" r:id="rId66" display="AS-PL"/>
+    <hyperlink ref="D65" r:id="rId63" display="Würth Electronic"/>
+    <hyperlink ref="D69" r:id="rId64" display="Farnell"/>
+    <hyperlink ref="F69" r:id="rId65" display="LEDEX"/>
+    <hyperlink ref="D70" r:id="rId66" display="Autodoc"/>
+    <hyperlink ref="F70" r:id="rId67" display="AS-PL"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3473,6 +3482,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId67"/>
+  <legacyDrawing r:id="rId68"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BOM.xlsx: Added UdeA components
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H21" authorId="0">
+    <comment ref="H22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H45" authorId="0">
+    <comment ref="H46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H50" authorId="0">
+    <comment ref="H52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="206">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -336,6 +336,18 @@
     <t xml:space="preserve">Raspberry Pi</t>
   </si>
   <si>
+    <t xml:space="preserve">Raspberry Pi RTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">713-103030277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry pi needs a real-time clock </t>
+  </si>
+  <si>
     <t xml:space="preserve">NUCLEO-H723ZG</t>
   </si>
   <si>
@@ -598,6 +610,18 @@
     <t xml:space="preserve">Break Beam sensor</t>
   </si>
   <si>
+    <t xml:space="preserve">APDS-9960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41013512 – Sparkfun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparkfun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB sensor chosen by UdeA for ball detection.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IR Break Beam Sensor - 5mm LEDs</t>
   </si>
   <si>
@@ -605,15 +629,6 @@
   </si>
   <si>
     <t xml:space="preserve">Break beam to detect if a ball is close (within a few mm) to the dribbler.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GY-9960-3.3 APDS-9960</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proto Supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGB sensor chosen by UdeA for ball detection.</t>
   </si>
   <si>
     <t xml:space="preserve">3D CAD and Mechanical</t>
@@ -826,7 +841,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -909,6 +924,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1040,7 +1062,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1173,15 +1195,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1381,10 +1407,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1911,11 +1937,11 @@
         <v>16</v>
       </c>
       <c r="K18" s="16" t="str">
-        <f aca="false">"Can be substituted with " &amp; BOM!B21</f>
+        <f aca="false">"Can be substituted with " &amp; BOM!B22</f>
         <v>Can be substituted with Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
         <v>1</v>
       </c>
@@ -1931,32 +1957,32 @@
       <c r="E19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>68</v>
+      <c r="F19" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="16" t="n">
+        <v>103030277</v>
       </c>
       <c r="H19" s="18" t="n">
-        <v>322.58</v>
+        <v>47.61</v>
       </c>
       <c r="I19" s="18" t="n">
-        <f aca="false">C19*H19</f>
-        <v>322.58</v>
+        <f aca="false">H19*C19</f>
+        <v>47.61</v>
       </c>
       <c r="J19" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="s">
-        <v>18</v>
+      <c r="K19" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="16" t="n">
         <v>1</v>
@@ -1965,31 +1991,31 @@
         <v>47</v>
       </c>
       <c r="E20" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>71</v>
-      </c>
       <c r="H20" s="18" t="n">
-        <v>181.82</v>
+        <v>322.58</v>
       </c>
       <c r="I20" s="18" t="n">
         <f aca="false">C20*H20</f>
-        <v>181.82</v>
+        <v>322.58</v>
       </c>
       <c r="J20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="K20" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="n">
-        <v>2</v>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>75</v>
@@ -1997,78 +2023,80 @@
       <c r="C21" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>65</v>
+      <c r="D21" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="16"/>
+      <c r="F21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="H21" s="18" t="n">
-        <v>729</v>
+        <v>181.82</v>
       </c>
       <c r="I21" s="18" t="n">
-        <f aca="false">H21*C21</f>
-        <v>729</v>
+        <f aca="false">C21*H21</f>
+        <v>181.82</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26"/>
-      <c r="B23" s="16" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="C22" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F22" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="18" t="n">
+        <v>729</v>
+      </c>
+      <c r="I22" s="18" t="n">
+        <f aca="false">H22*C22</f>
+        <v>729</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23" s="18" t="n">
-        <v>75.44</v>
-      </c>
-      <c r="I23" s="18" t="n">
-        <f aca="false">C23*H23</f>
-        <v>75.44</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="16" t="s">
+    </row>
+    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26"/>
@@ -2088,203 +2116,201 @@
         <v>85</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H24" s="18" t="n">
-        <v>40.48</v>
+        <v>75.44</v>
       </c>
       <c r="I24" s="18" t="n">
         <f aca="false">C24*H24</f>
-        <v>40.48</v>
+        <v>75.44</v>
       </c>
       <c r="J24" s="16" t="s">
         <v>16</v>
       </c>
       <c r="K24" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="26"/>
+      <c r="B25" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="C25" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="16" t="s">
+      <c r="F25" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17" t="s">
+      <c r="G25" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="18" t="n">
+        <v>40.48</v>
+      </c>
+      <c r="I25" s="18" t="n">
+        <f aca="false">C25*H25</f>
+        <v>40.48</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E27" s="16" t="n">
         <v>63197</v>
       </c>
-      <c r="F26" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" s="18" t="n">
+      <c r="F27" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="18" t="n">
         <v>351.2</v>
-      </c>
-      <c r="I26" s="18" t="n">
-        <f aca="false">C26*H26</f>
-        <v>351.2</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="16" t="n">
-        <v>433122</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="18" t="n">
-        <v>359.2</v>
       </c>
       <c r="I27" s="18" t="n">
         <f aca="false">C27*H27</f>
-        <v>359.2</v>
+        <v>351.2</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>16</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="B28" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="16" t="n">
+        <v>433122</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="18" t="n">
+        <v>359.2</v>
+      </c>
+      <c r="I28" s="18" t="n">
+        <f aca="false">C28*H28</f>
+        <v>359.2</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K30" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H30" s="18" t="n">
-        <v>117.54</v>
-      </c>
-      <c r="I30" s="18" t="n">
-        <f aca="false">H30*C30</f>
-        <v>117.54</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="C31" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>101</v>
@@ -2293,14 +2319,14 @@
         <v>102</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H31" s="18" t="n">
-        <v>98.56</v>
+        <v>117.54</v>
       </c>
       <c r="I31" s="18" t="n">
         <f aca="false">H31*C31</f>
-        <v>98.56</v>
+        <v>117.54</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>16</v>
@@ -2317,10 +2343,10 @@
         <v>104</v>
       </c>
       <c r="C32" s="16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>105</v>
@@ -2332,11 +2358,11 @@
         <v>104</v>
       </c>
       <c r="H32" s="18" t="n">
-        <v>4.09</v>
+        <v>98.56</v>
       </c>
       <c r="I32" s="18" t="n">
-        <f aca="false">C32*H32</f>
-        <v>8.18</v>
+        <f aca="false">H32*C32</f>
+        <v>98.56</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>16</v>
@@ -2346,26 +2372,49 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28"/>
+      <c r="A33" s="22" t="n">
+        <v>1</v>
+      </c>
       <c r="B33" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C33" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H33" s="18" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="I33" s="18" t="n">
+        <f aca="false">C33*H33</f>
+        <v>8.18</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
+      <c r="B34" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="16" t="n">
+        <v>10</v>
+      </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
@@ -2375,344 +2424,321 @@
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="4" t="s">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="28"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="I37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="16" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H38" s="18" t="n">
-        <v>224.4</v>
-      </c>
-      <c r="I38" s="18" t="n">
-        <f aca="false">C38*H38</f>
-        <v>897.6</v>
-      </c>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16" t="s">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="C39" s="16" t="n">
         <v>4</v>
       </c>
       <c r="D39" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="25"/>
+      <c r="F39" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H39" s="18" t="n">
+        <v>224.4</v>
+      </c>
+      <c r="I39" s="18" t="n">
+        <f aca="false">C39*H39</f>
+        <v>897.6</v>
+      </c>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39" s="18" t="n">
+      <c r="E40" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H40" s="18" t="n">
         <v>197.69</v>
       </c>
-      <c r="I39" s="18" t="n">
-        <f aca="false">H39*C39</f>
+      <c r="I40" s="18" t="n">
+        <f aca="false">H40*C40</f>
         <v>790.76</v>
       </c>
-      <c r="J39" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="K39" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="n">
+      <c r="J40" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B40" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" s="16" t="n">
+      <c r="B41" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D41" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="H40" s="18" t="n">
+      <c r="E41" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41" s="18" t="n">
         <v>309</v>
-      </c>
-      <c r="I40" s="18" t="n">
-        <f aca="false">C40*H40</f>
-        <v>2472</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="K40" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="H41" s="18" t="n">
-        <v>198.352</v>
       </c>
       <c r="I41" s="18" t="n">
         <f aca="false">C41*H41</f>
+        <v>2472</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" s="18" t="n">
+        <v>198.352</v>
+      </c>
+      <c r="I42" s="18" t="n">
+        <f aca="false">C42*H42</f>
         <v>793.408</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J42" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K41" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="16" t="n">
+      <c r="K42" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="G43" s="16" t="n">
+      <c r="D44" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="16"/>
+      <c r="F44" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="16" t="n">
         <v>2536030320001</v>
       </c>
-      <c r="H43" s="18" t="n">
+      <c r="H44" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="I43" s="18" t="n">
-        <f aca="false">C43*H43</f>
+      <c r="I44" s="18" t="n">
+        <f aca="false">C44*H44</f>
         <v>0</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J44" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K43" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C45" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" s="17" t="s">
+      <c r="K44" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" s="17" t="s">
+      <c r="E46" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="18" t="n">
+      <c r="G46" s="16"/>
+      <c r="H46" s="18" t="n">
         <v>369</v>
-      </c>
-      <c r="I45" s="18" t="n">
-        <f aca="false">H45*C45</f>
-        <v>369</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="31" t="str">
-        <f aca="false">"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B21</f>
-        <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H46" s="18" t="n">
-        <v>176.32</v>
       </c>
       <c r="I46" s="18" t="n">
         <f aca="false">H46*C46</f>
-        <v>176.32</v>
+        <v>369</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="31" t="s">
-        <v>144</v>
+      <c r="K46" s="31" t="str">
+        <f aca="false">"Needs to be ordered with " &amp; BOM!B18 &amp; "or " &amp; BOM!B22</f>
+        <v>Needs to be ordered with Raspberry Pi 4 Model B/8GB or Raspberry Pi 4 Model B/4GB</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,29 +2746,29 @@
         <v>18</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C47" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="F47" s="32" t="s">
-        <v>142</v>
+      <c r="F47" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>147</v>
       </c>
       <c r="H47" s="18" t="n">
-        <v>39.62</v>
+        <v>176.32</v>
       </c>
       <c r="I47" s="18" t="n">
         <f aca="false">H47*C47</f>
-        <v>39.62</v>
+        <v>176.32</v>
       </c>
       <c r="J47" s="16" t="s">
         <v>16</v>
@@ -2752,8 +2778,8 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="20" t="n">
-        <v>3</v>
+      <c r="A48" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>149</v>
@@ -2762,189 +2788,216 @@
         <v>1</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F48" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="G48" s="16" t="s">
-        <v>152</v>
-      </c>
       <c r="H48" s="18" t="n">
-        <v>605.13</v>
+        <v>39.62</v>
       </c>
       <c r="I48" s="18" t="n">
-        <f aca="false">C48*H48</f>
-        <v>605.13</v>
+        <f aca="false">H48*C48</f>
+        <v>39.62</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K48" s="16" t="s">
+      <c r="K48" s="31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+      <c r="C49" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B50" s="16" t="s">
+      <c r="F49" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="C50" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="25" t="s">
+      <c r="G49" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H49" s="18" t="n">
+        <v>605.13</v>
+      </c>
+      <c r="I49" s="18" t="n">
+        <f aca="false">C49*H49</f>
+        <v>605.13</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="16" t="n">
+      <c r="E51" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F51" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" s="18" t="n">
+        <v>199</v>
+      </c>
+      <c r="I51" s="18" t="n">
+        <v>199</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="16" t="n">
         <v>41015028</v>
       </c>
-      <c r="F50" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" s="16"/>
-      <c r="H50" s="18" t="n">
+      <c r="F52" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="18" t="n">
         <v>99</v>
       </c>
-      <c r="I50" s="18" t="n">
-        <f aca="false">H50*C50</f>
+      <c r="I52" s="18" t="n">
+        <f aca="false">H52*C52</f>
         <v>99</v>
       </c>
-      <c r="J50" s="16" t="s">
+      <c r="J52" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K50" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="18" t="n">
-        <v>44.8</v>
-      </c>
-      <c r="I51" s="18" t="n">
-        <v>44.8</v>
-      </c>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="16"/>
-      <c r="B53" s="4" t="s">
+      <c r="K52" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="16"/>
+      <c r="B54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="G54" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H54" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="5" t="s">
+      <c r="I54" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K53" s="4" t="s">
+      <c r="K54" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="28"/>
-      <c r="B55" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="28"/>
       <c r="B56" s="16" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
@@ -2954,14 +3007,12 @@
       <c r="H56" s="18"/>
       <c r="I56" s="18"/>
       <c r="J56" s="16"/>
-      <c r="K56" s="16" t="s">
-        <v>164</v>
-      </c>
+      <c r="K56" s="16"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28"/>
       <c r="B57" s="16" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
@@ -2972,13 +3023,13 @@
       <c r="I57" s="18"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28"/>
       <c r="B58" s="16" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
@@ -2989,13 +3040,13 @@
       <c r="I58" s="18"/>
       <c r="J58" s="16"/>
       <c r="K58" s="16" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28"/>
       <c r="B59" s="16" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
@@ -3006,99 +3057,87 @@
       <c r="I59" s="18"/>
       <c r="J59" s="16"/>
       <c r="K59" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="22" t="n">
-        <v>1</v>
-      </c>
+      <c r="A60" s="28"/>
       <c r="B60" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="E60" s="16" t="n">
-        <v>41019265</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
-      <c r="H60" s="18" t="n">
-        <v>18</v>
-      </c>
-      <c r="I60" s="18" t="n">
-        <f aca="false">C60*H60</f>
-        <v>72</v>
-      </c>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
       <c r="J60" s="16"/>
       <c r="K60" s="16" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-    </row>
-    <row r="62" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="28"/>
-      <c r="B62" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C62" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E62" s="33" t="n">
-        <v>173010335</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G62" s="16"/>
-      <c r="H62" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I62" s="18"/>
-      <c r="J62" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K62" s="16" t="s">
         <v>173</v>
       </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E61" s="16" t="n">
+        <v>41019265</v>
+      </c>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="I61" s="18" t="n">
+        <f aca="false">C61*H61</f>
+        <v>72</v>
+      </c>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28"/>
       <c r="B63" s="16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C63" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E63" s="33" t="n">
-        <v>173010542</v>
+        <v>137</v>
+      </c>
+      <c r="E63" s="34" t="n">
+        <v>173010335</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="18" t="n">
@@ -3109,25 +3148,25 @@
         <v>16</v>
       </c>
       <c r="K63" s="16" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28"/>
       <c r="B64" s="16" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C64" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="16" t="n">
-        <v>173011235</v>
+        <v>137</v>
+      </c>
+      <c r="E64" s="34" t="n">
+        <v>173010542</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="18" t="n">
@@ -3138,25 +3177,25 @@
         <v>16</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28"/>
       <c r="B65" s="16" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C65" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E65" s="33" t="n">
-        <v>173011535</v>
+        <v>137</v>
+      </c>
+      <c r="E65" s="16" t="n">
+        <v>173011235</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G65" s="16"/>
       <c r="H65" s="18" t="n">
@@ -3167,120 +3206,115 @@
         <v>16</v>
       </c>
       <c r="K65" s="16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="16"/>
-      <c r="B67" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="28"/>
+      <c r="B66" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" s="34" t="n">
+        <v>173011535</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G66" s="16"/>
+      <c r="H66" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="18"/>
+      <c r="J66" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K66" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="16"/>
+      <c r="B68" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F68" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G68" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H68" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I68" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="J68" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K67" s="4" t="s">
+      <c r="K68" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="C69" s="16" t="n">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C70" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="D70" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="H69" s="18" t="n">
-        <v>262.83</v>
-      </c>
-      <c r="I69" s="18" t="n">
-        <f aca="false">C69*H69</f>
-        <v>1576.98</v>
-      </c>
-      <c r="J69" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K69" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="15"/>
-      <c r="B70" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C70" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="E70" s="16" t="n">
-        <v>5901259432770</v>
-      </c>
+      <c r="E70" s="16"/>
       <c r="F70" s="17" t="s">
         <v>185</v>
       </c>
@@ -3288,96 +3322,127 @@
         <v>186</v>
       </c>
       <c r="H70" s="18" t="n">
-        <v>237</v>
+        <v>262.83</v>
       </c>
       <c r="I70" s="18" t="n">
         <f aca="false">C70*H70</f>
-        <v>237</v>
+        <v>1576.98</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K70" s="16"/>
-    </row>
-    <row r="74" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="34" t="s">
+      <c r="K70" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="35" t="n">
-        <f aca="false">SUM(I4,I10,I14,I18,I19,I23,I24,I26,I29,I38,I45,I50,I60)</f>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15"/>
+      <c r="B71" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="16" t="n">
+        <v>5901259432770</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="H71" s="18" t="n">
+        <v>237</v>
+      </c>
+      <c r="I71" s="18" t="n">
+        <f aca="false">C71*H71</f>
+        <v>237</v>
+      </c>
+      <c r="J71" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="16"/>
+    </row>
+    <row r="75" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C75" s="36" t="n">
+        <f aca="false">SUM(I4,I10,I14,I18,I20,I24,I25,I27,I30,I39,I46,I52,I61)</f>
         <v>7699.9</v>
       </c>
-      <c r="E74" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="F74" s="36"/>
-      <c r="G74" s="37" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="F75" s="22"/>
-      <c r="G75" s="16" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="16" t="s">
+      <c r="E75" s="37" t="s">
         <v>193</v>
       </c>
+      <c r="F75" s="37"/>
+      <c r="G75" s="38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="39" t="s">
+        <v>195</v>
+      </c>
       <c r="E76" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="F76" s="15"/>
-      <c r="G76" s="16"/>
+        <v>196</v>
+      </c>
+      <c r="F76" s="22"/>
+      <c r="G76" s="16" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="16" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F77" s="20"/>
+        <v>199</v>
+      </c>
+      <c r="F77" s="15"/>
       <c r="G77" s="16"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="16" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F78" s="28"/>
+        <v>200</v>
+      </c>
+      <c r="F78" s="20"/>
+      <c r="G78" s="16"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="16" t="s">
-        <v>198</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F79" s="28"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="16" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="16" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="31"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="16" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="31"/>
@@ -3385,6 +3450,10 @@
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="31"/>
     </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="31"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="A1:K1"/>
@@ -3392,20 +3461,20 @@
     <mergeCell ref="A9:K9"/>
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A28:K28"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A61:K61"/>
-    <mergeCell ref="A66:K66"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="A62:K62"/>
+    <mergeCell ref="A67:K67"/>
+    <mergeCell ref="A69:K69"/>
+    <mergeCell ref="E75:F75"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId2" display="Nanotec"/>
@@ -3428,52 +3497,55 @@
     <hyperlink ref="D18" r:id="rId19" display="Electro:kit"/>
     <hyperlink ref="F18" r:id="rId20" display="Raspberry Pi"/>
     <hyperlink ref="D19" r:id="rId21" display="Mouser"/>
-    <hyperlink ref="F19" r:id="rId22" display="STMicroelectronics"/>
+    <hyperlink ref="F19" r:id="rId22" display="Seeed"/>
     <hyperlink ref="D20" r:id="rId23" display="Mouser"/>
-    <hyperlink ref="F20" r:id="rId24" display="Espressif Systems"/>
-    <hyperlink ref="D21" r:id="rId25" display="Electro:kit"/>
-    <hyperlink ref="D23" r:id="rId26" display="Mouser"/>
-    <hyperlink ref="F23" r:id="rId27" display="Semtech"/>
+    <hyperlink ref="F20" r:id="rId24" display="STMicroelectronics"/>
+    <hyperlink ref="D21" r:id="rId25" display="Mouser"/>
+    <hyperlink ref="F21" r:id="rId26" display="Espressif Systems"/>
+    <hyperlink ref="D22" r:id="rId27" display="Electro:kit"/>
     <hyperlink ref="D24" r:id="rId28" display="Mouser"/>
-    <hyperlink ref="F24" r:id="rId29" display="Skyworks Solutions, Inc."/>
-    <hyperlink ref="D26" r:id="rId30" display="Elefun"/>
-    <hyperlink ref="F26" r:id="rId31" display="GNB"/>
-    <hyperlink ref="D27" r:id="rId32" display="Droneit"/>
-    <hyperlink ref="D30" r:id="rId33" display="DigiKey"/>
-    <hyperlink ref="F30" r:id="rId34" display="Analog Devices Inc."/>
-    <hyperlink ref="D31" r:id="rId35" display="Mouser"/>
-    <hyperlink ref="F31" r:id="rId36" display="Coilcraft"/>
-    <hyperlink ref="D32" r:id="rId37" display="DigiKey"/>
-    <hyperlink ref="F32" r:id="rId38" display="Diodes Incorporated"/>
-    <hyperlink ref="D38" r:id="rId39" display="Symmetry Electronics"/>
-    <hyperlink ref="F38" r:id="rId40" location="documents" display="iC-Haus"/>
-    <hyperlink ref="D39" r:id="rId41" display="Mouser"/>
-    <hyperlink ref="F39" r:id="rId42" display="ams OSRAM"/>
-    <hyperlink ref="D40" r:id="rId43" display="Farnell"/>
-    <hyperlink ref="F40" r:id="rId44" display="BROADCOM"/>
-    <hyperlink ref="D41" r:id="rId45" display="Mouser"/>
-    <hyperlink ref="F41" r:id="rId46" display="Same sky"/>
-    <hyperlink ref="D43" r:id="rId47" display="Würth Electronic"/>
-    <hyperlink ref="F43" r:id="rId48" display="Würth Elektronik"/>
-    <hyperlink ref="D45" r:id="rId49" display="Electro:kit"/>
-    <hyperlink ref="F45" r:id="rId50" display="Raspberry Pi"/>
-    <hyperlink ref="D46" r:id="rId51" display="Amazon.com"/>
-    <hyperlink ref="F46" r:id="rId52" display="STmicroelectronics"/>
-    <hyperlink ref="D47" r:id="rId53" display="Tiny tronics"/>
+    <hyperlink ref="F24" r:id="rId29" display="Semtech"/>
+    <hyperlink ref="D25" r:id="rId30" display="Mouser"/>
+    <hyperlink ref="F25" r:id="rId31" display="Skyworks Solutions, Inc."/>
+    <hyperlink ref="D27" r:id="rId32" display="Elefun"/>
+    <hyperlink ref="F27" r:id="rId33" display="GNB"/>
+    <hyperlink ref="D28" r:id="rId34" display="Droneit"/>
+    <hyperlink ref="D31" r:id="rId35" display="DigiKey"/>
+    <hyperlink ref="F31" r:id="rId36" display="Analog Devices Inc."/>
+    <hyperlink ref="D32" r:id="rId37" display="Mouser"/>
+    <hyperlink ref="F32" r:id="rId38" display="Coilcraft"/>
+    <hyperlink ref="D33" r:id="rId39" display="DigiKey"/>
+    <hyperlink ref="F33" r:id="rId40" display="Diodes Incorporated"/>
+    <hyperlink ref="D39" r:id="rId41" display="Symmetry Electronics"/>
+    <hyperlink ref="F39" r:id="rId42" location="documents" display="iC-Haus"/>
+    <hyperlink ref="D40" r:id="rId43" display="Mouser"/>
+    <hyperlink ref="F40" r:id="rId44" display="ams OSRAM"/>
+    <hyperlink ref="D41" r:id="rId45" display="Farnell"/>
+    <hyperlink ref="F41" r:id="rId46" display="BROADCOM"/>
+    <hyperlink ref="D42" r:id="rId47" display="Mouser"/>
+    <hyperlink ref="F42" r:id="rId48" display="Same sky"/>
+    <hyperlink ref="D44" r:id="rId49" display="Würth Electronic"/>
+    <hyperlink ref="F44" r:id="rId50" display="Würth Elektronik"/>
+    <hyperlink ref="D46" r:id="rId51" display="Electro:kit"/>
+    <hyperlink ref="F46" r:id="rId52" display="Raspberry Pi"/>
+    <hyperlink ref="D47" r:id="rId53" display="Amazon.com"/>
     <hyperlink ref="F47" r:id="rId54" display="STmicroelectronics"/>
-    <hyperlink ref="D48" r:id="rId55" display="Mouser"/>
-    <hyperlink ref="F48" r:id="rId56" display="Texas Instruments"/>
-    <hyperlink ref="D50" r:id="rId57" display="Electro:kit"/>
-    <hyperlink ref="D51" r:id="rId58" display="Proto Supplies"/>
-    <hyperlink ref="D60" r:id="rId59" display="Electrokit"/>
-    <hyperlink ref="D62" r:id="rId60" display="Würth Electronic"/>
-    <hyperlink ref="D63" r:id="rId61" display="Würth Electronic"/>
-    <hyperlink ref="D64" r:id="rId62" display="Würth Electronic"/>
-    <hyperlink ref="D65" r:id="rId63" display="Würth Electronic"/>
-    <hyperlink ref="D69" r:id="rId64" display="Farnell"/>
-    <hyperlink ref="F69" r:id="rId65" display="LEDEX"/>
-    <hyperlink ref="D70" r:id="rId66" display="Autodoc"/>
-    <hyperlink ref="F70" r:id="rId67" display="AS-PL"/>
+    <hyperlink ref="D48" r:id="rId55" display="Tiny tronics"/>
+    <hyperlink ref="F48" r:id="rId56" display="STmicroelectronics"/>
+    <hyperlink ref="D49" r:id="rId57" display="Mouser"/>
+    <hyperlink ref="F49" r:id="rId58" display="Texas Instruments"/>
+    <hyperlink ref="D51" r:id="rId59" display="Electro:kit"/>
+    <hyperlink ref="F51" r:id="rId60" display="Sparkfun"/>
+    <hyperlink ref="D52" r:id="rId61" display="Electro:kit"/>
+    <hyperlink ref="D61" r:id="rId62" display="Electrokit"/>
+    <hyperlink ref="D63" r:id="rId63" display="Würth Electronic"/>
+    <hyperlink ref="D64" r:id="rId64" display="Würth Electronic"/>
+    <hyperlink ref="D65" r:id="rId65" display="Würth Electronic"/>
+    <hyperlink ref="D66" r:id="rId66" display="Würth Electronic"/>
+    <hyperlink ref="D70" r:id="rId67" display="Farnell"/>
+    <hyperlink ref="F70" r:id="rId68" display="LEDEX"/>
+    <hyperlink ref="D71" r:id="rId69" display="Autodoc"/>
+    <hyperlink ref="F71" r:id="rId70" display="AS-PL"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3482,6 +3554,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId68"/>
+  <legacyDrawing r:id="rId71"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BOM.xlsx: Added connectors section
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="207">
   <si>
     <t xml:space="preserve">Powertrain and Electronics</t>
   </si>
@@ -677,6 +677,9 @@
   </si>
   <si>
     <t xml:space="preserve">Voltage regulator (buck converters) -&gt; 15V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors</t>
   </si>
   <si>
     <t xml:space="preserve">Actuators</t>
@@ -841,7 +844,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -924,13 +927,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1195,19 +1191,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1407,10 +1403,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2880,7 +2876,7 @@
       <c r="E51" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="F51" s="33" t="s">
+      <c r="F51" s="17" t="s">
         <v>161</v>
       </c>
       <c r="G51" s="16" t="s">
@@ -3133,7 +3129,7 @@
       <c r="D63" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E63" s="34" t="n">
+      <c r="E63" s="33" t="n">
         <v>173010335</v>
       </c>
       <c r="F63" s="16" t="s">
@@ -3162,7 +3158,7 @@
       <c r="D64" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E64" s="34" t="n">
+      <c r="E64" s="33" t="n">
         <v>173010542</v>
       </c>
       <c r="F64" s="16" t="s">
@@ -3220,7 +3216,7 @@
       <c r="D66" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E66" s="34" t="n">
+      <c r="E66" s="33" t="n">
         <v>173011535</v>
       </c>
       <c r="F66" s="16" t="s">
@@ -3238,205 +3234,223 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16"/>
-      <c r="B68" s="4" t="s">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="34"/>
+    </row>
+    <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="16"/>
+      <c r="B70" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F70" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G68" s="4" t="s">
+      <c r="G70" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H70" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I70" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J68" s="4" t="s">
+      <c r="J70" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K68" s="4" t="s">
+      <c r="K70" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B70" s="16" t="s">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C70" s="16" t="n">
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="D70" s="17" t="s">
+      <c r="D72" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="16"/>
-      <c r="F70" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G70" s="16" t="s">
+      <c r="E72" s="16"/>
+      <c r="F72" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="H70" s="18" t="n">
+      <c r="G72" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H72" s="18" t="n">
         <v>262.83</v>
       </c>
-      <c r="I70" s="18" t="n">
-        <f aca="false">C70*H70</f>
+      <c r="I72" s="18" t="n">
+        <f aca="false">C72*H72</f>
         <v>1576.98</v>
       </c>
-      <c r="J70" s="16" t="s">
+      <c r="J72" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K70" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="15"/>
-      <c r="B71" s="19" t="s">
+      <c r="K72" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="C71" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D71" s="17" t="s">
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="15"/>
+      <c r="B73" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="E71" s="16" t="n">
+      <c r="C73" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E73" s="16" t="n">
         <v>5901259432770</v>
       </c>
-      <c r="F71" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="G71" s="16" t="s">
+      <c r="F73" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="H71" s="18" t="n">
+      <c r="G73" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="H73" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="I71" s="18" t="n">
-        <f aca="false">C71*H71</f>
+      <c r="I73" s="18" t="n">
+        <f aca="false">C73*H73</f>
         <v>237</v>
       </c>
-      <c r="J71" s="16" t="s">
+      <c r="J73" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K71" s="16"/>
-    </row>
-    <row r="75" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C75" s="36" t="n">
+      <c r="K73" s="16"/>
+    </row>
+    <row r="77" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="36" t="n">
         <f aca="false">SUM(I4,I10,I14,I18,I20,I24,I25,I27,I30,I39,I46,I52,I61)</f>
         <v>7699.9</v>
       </c>
-      <c r="E75" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="F75" s="37"/>
-      <c r="G75" s="38" t="s">
+      <c r="E77" s="37" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="39" t="s">
+      <c r="F77" s="37"/>
+      <c r="G77" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="E76" s="16" t="s">
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="F76" s="22"/>
-      <c r="G76" s="16" t="s">
+      <c r="E78" s="16" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="16" t="s">
+      <c r="F78" s="22"/>
+      <c r="G78" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="E77" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="F78" s="20"/>
-      <c r="G78" s="16"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="F79" s="28"/>
+        <v>200</v>
+      </c>
+      <c r="F79" s="15"/>
+      <c r="G79" s="16"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="16" t="s">
-        <v>203</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F80" s="20"/>
+      <c r="G80" s="16"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="16" t="s">
-        <v>204</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="F81" s="28"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="16" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3444,18 +3458,27 @@
         <v>205</v>
       </c>
     </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="31"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="31"/>
+      <c r="B85" s="16" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="31"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="31"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="31"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A9:K9"/>
@@ -3474,7 +3497,8 @@
     <mergeCell ref="A62:K62"/>
     <mergeCell ref="A67:K67"/>
     <mergeCell ref="A69:K69"/>
-    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="E77:F77"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId2" display="Nanotec"/>
@@ -3542,10 +3566,10 @@
     <hyperlink ref="D64" r:id="rId64" display="Würth Electronic"/>
     <hyperlink ref="D65" r:id="rId65" display="Würth Electronic"/>
     <hyperlink ref="D66" r:id="rId66" display="Würth Electronic"/>
-    <hyperlink ref="D70" r:id="rId67" display="Farnell"/>
-    <hyperlink ref="F70" r:id="rId68" display="LEDEX"/>
-    <hyperlink ref="D71" r:id="rId69" display="Autodoc"/>
-    <hyperlink ref="F71" r:id="rId70" display="AS-PL"/>
+    <hyperlink ref="D72" r:id="rId67" display="Farnell"/>
+    <hyperlink ref="F72" r:id="rId68" display="LEDEX"/>
+    <hyperlink ref="D73" r:id="rId69" display="Autodoc"/>
+    <hyperlink ref="F73" r:id="rId70" display="AS-PL"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>